<commit_message>
finished api and excel
</commit_message>
<xml_diff>
--- a/gpt-dmn-evaluation.xlsx
+++ b/gpt-dmn-evaluation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eduhtlklu-my.sharepoint.com/personal/marcel_ewinger_alumni_htl-klu_at/Documents/Uni/Master/2.Semester/Information Systems Engineering/Project/GPT-4-for-Decision-Logic-Modeling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="8_{A43CEE57-BBAA-4F95-ACC3-1D1EE3724512}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B2287405-33E0-4B4C-8F10-72D94E777951}"/>
+  <xr:revisionPtr revIDLastSave="334" documentId="8_{A43CEE57-BBAA-4F95-ACC3-1D1EE3724512}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F0B2C8B5-F151-4316-8093-9AD609277045}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2074" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2075" uniqueCount="47">
   <si>
     <t>Temp</t>
   </si>
@@ -173,6 +173,9 @@
   <si>
     <t>STDV of MEAN</t>
   </si>
+  <si>
+    <t>Accuracy</t>
+  </si>
 </sst>
 </file>
 
@@ -181,7 +184,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -189,16 +192,37 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -248,11 +272,91 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -282,6 +386,40 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -297,6 +435,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -598,12 +740,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96D64403-17FB-468D-8303-A84CFBCA623E}">
   <dimension ref="B7:AA314"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="J40" sqref="J40"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="W138" sqref="W138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="4" max="4" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="1.88671875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6807,15 +6950,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B4C4489-1E2D-4E6E-9C7F-DB4F704F54BF}">
-  <dimension ref="B7:AA314"/>
+  <dimension ref="B7:AF314"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="T9" sqref="T9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q139" sqref="Q139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="4" max="4" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="10" width="9.44140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="1.88671875" customWidth="1"/>
+    <col min="12" max="14" width="9.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="7" spans="2:27" ht="43.2" x14ac:dyDescent="0.3">
@@ -7023,28 +7169,36 @@
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="7">
-        <v>1</v>
-      </c>
-      <c r="G12" s="9">
-        <v>0</v>
-      </c>
-      <c r="H12" s="9">
-        <v>1</v>
-      </c>
-      <c r="I12" s="9">
-        <v>1</v>
-      </c>
-      <c r="J12" s="9">
-        <v>0</v>
-      </c>
-      <c r="K12" s="9"/>
-      <c r="L12" s="9">
-        <v>1</v>
-      </c>
-      <c r="M12" s="9">
-        <v>1</v>
-      </c>
-      <c r="N12" s="9">
+        <f>COUNTIF(F9:F11,"Y")/3</f>
+        <v>1</v>
+      </c>
+      <c r="G12" s="7">
+        <f>COUNTIF(G9:G11,"Y")/3</f>
+        <v>0</v>
+      </c>
+      <c r="H12" s="7">
+        <f t="shared" ref="H12:N12" si="0">COUNTIF(H9:H11,"Y")/3</f>
+        <v>1</v>
+      </c>
+      <c r="I12" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J12" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="M12" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="N12" s="7">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="W12">
@@ -7143,15 +7297,19 @@
       <c r="V14" s="2"/>
       <c r="W14" s="2"/>
       <c r="X14" s="7">
-        <v>0</v>
-      </c>
-      <c r="Y14" s="9">
-        <v>1</v>
-      </c>
-      <c r="Z14" s="9">
-        <v>0</v>
-      </c>
-      <c r="AA14" s="9">
+        <f>COUNTIF(X11:X13,"Y")/3</f>
+        <v>0</v>
+      </c>
+      <c r="Y14" s="7">
+        <f t="shared" ref="Y14:AA14" si="1">COUNTIF(Y11:Y13,"Y")/3</f>
+        <v>1</v>
+      </c>
+      <c r="Z14" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AA14" s="7">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -7207,28 +7365,36 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="7">
-        <v>1</v>
-      </c>
-      <c r="G16" s="9">
-        <v>0</v>
-      </c>
-      <c r="H16" s="9">
-        <v>1</v>
-      </c>
-      <c r="I16" s="9">
-        <v>0.33</v>
-      </c>
-      <c r="J16" s="9">
-        <v>0.33</v>
-      </c>
-      <c r="K16" s="9"/>
-      <c r="L16" s="9">
-        <v>0.67</v>
-      </c>
-      <c r="M16" s="9">
-        <v>0.67</v>
-      </c>
-      <c r="N16" s="9">
+        <f>COUNTIF(F13:F15,"Y")/3</f>
+        <v>1</v>
+      </c>
+      <c r="G16" s="7">
+        <f t="shared" ref="G16:N16" si="2">COUNTIF(G13:G15,"Y")/3</f>
+        <v>0</v>
+      </c>
+      <c r="H16" s="7">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="I16" s="7">
+        <f t="shared" si="2"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="J16" s="7">
+        <f t="shared" si="2"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7">
+        <f t="shared" si="2"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="M16" s="7">
+        <f t="shared" si="2"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="N16" s="7">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="W16">
@@ -7327,15 +7493,19 @@
       <c r="V18" s="2"/>
       <c r="W18" s="2"/>
       <c r="X18" s="7">
-        <v>0</v>
-      </c>
-      <c r="Y18" s="9">
-        <v>0.67</v>
-      </c>
-      <c r="Z18" s="9">
-        <v>0</v>
-      </c>
-      <c r="AA18" s="9">
+        <f>COUNTIF(X15:X17,"Y")/3</f>
+        <v>0</v>
+      </c>
+      <c r="Y18" s="7">
+        <f t="shared" ref="Y18:AA18" si="3">COUNTIF(Y15:Y17,"Y")/3</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="Z18" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AA18" s="7">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -7391,28 +7561,36 @@
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="7">
-        <v>1</v>
-      </c>
-      <c r="G20" s="9">
-        <v>0</v>
-      </c>
-      <c r="H20" s="9">
-        <v>0.67</v>
-      </c>
-      <c r="I20" s="9">
-        <v>0.67</v>
-      </c>
-      <c r="J20" s="9">
-        <v>0.33</v>
-      </c>
-      <c r="K20" s="9"/>
-      <c r="L20" s="9">
-        <v>0.67</v>
-      </c>
-      <c r="M20" s="9">
-        <v>1</v>
-      </c>
-      <c r="N20" s="9">
+        <f>COUNTIF(F17:F19,"Y")/3</f>
+        <v>1</v>
+      </c>
+      <c r="G20" s="7">
+        <f t="shared" ref="G20:N20" si="4">COUNTIF(G17:G19,"Y")/3</f>
+        <v>0</v>
+      </c>
+      <c r="H20" s="7">
+        <f t="shared" si="4"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="I20" s="7">
+        <f t="shared" si="4"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="J20" s="7">
+        <f t="shared" si="4"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7">
+        <f t="shared" si="4"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="M20" s="7">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="N20" s="7">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="W20">
@@ -7511,15 +7689,19 @@
       <c r="V22" s="2"/>
       <c r="W22" s="2"/>
       <c r="X22" s="7">
-        <v>0</v>
-      </c>
-      <c r="Y22" s="9">
-        <v>1</v>
-      </c>
-      <c r="Z22" s="9">
-        <v>0</v>
-      </c>
-      <c r="AA22" s="9">
+        <f>COUNTIF(X19:X21,"Y")/3</f>
+        <v>0</v>
+      </c>
+      <c r="Y22" s="7">
+        <f t="shared" ref="Y22:AA22" si="5">COUNTIF(Y19:Y21,"Y")/3</f>
+        <v>1</v>
+      </c>
+      <c r="Z22" s="7">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AA22" s="7">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -7575,28 +7757,36 @@
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
       <c r="F24" s="7">
-        <v>1</v>
-      </c>
-      <c r="G24" s="9">
-        <v>0.67</v>
-      </c>
-      <c r="H24" s="9">
-        <v>1</v>
-      </c>
-      <c r="I24" s="9">
-        <v>1</v>
-      </c>
-      <c r="J24" s="9">
-        <v>0.33</v>
-      </c>
-      <c r="K24" s="9"/>
-      <c r="L24" s="9">
-        <v>0</v>
-      </c>
-      <c r="M24" s="9">
-        <v>0.67</v>
-      </c>
-      <c r="N24" s="9">
+        <f>COUNTIF(F21:F23,"Y")/3</f>
+        <v>1</v>
+      </c>
+      <c r="G24" s="7">
+        <f t="shared" ref="G24:N24" si="6">COUNTIF(G21:G23,"Y")/3</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="H24" s="7">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="I24" s="7">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="J24" s="7">
+        <f t="shared" si="6"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="K24" s="7"/>
+      <c r="L24" s="7">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M24" s="7">
+        <f t="shared" si="6"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="N24" s="7">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="W24">
@@ -7621,28 +7811,36 @@
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="6">
-        <v>1</v>
-      </c>
-      <c r="G25" s="8">
-        <v>0.16700000000000001</v>
-      </c>
-      <c r="H25" s="8">
-        <v>0.91700000000000004</v>
-      </c>
-      <c r="I25" s="8">
+        <f>AVERAGE(F9:F24)</f>
+        <v>1</v>
+      </c>
+      <c r="G25" s="6">
+        <f t="shared" ref="G25:N25" si="7">AVERAGE(G9:G24)</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="H25" s="6">
+        <f t="shared" si="7"/>
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="I25" s="6">
+        <f t="shared" si="7"/>
         <v>0.75</v>
       </c>
-      <c r="J25" s="8">
+      <c r="J25" s="6">
+        <f t="shared" si="7"/>
         <v>0.25</v>
       </c>
-      <c r="K25" s="8"/>
-      <c r="L25" s="8">
-        <v>0.58299999999999996</v>
-      </c>
-      <c r="M25" s="8">
-        <v>0.83299999999999996</v>
-      </c>
-      <c r="N25" s="8">
+      <c r="K25" s="6"/>
+      <c r="L25" s="6">
+        <f t="shared" si="7"/>
+        <v>0.58333333333333326</v>
+      </c>
+      <c r="M25" s="6">
+        <f t="shared" si="7"/>
+        <v>0.83333333333333326</v>
+      </c>
+      <c r="N25" s="6">
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="W25">
@@ -7665,33 +7863,41 @@
       <c r="V26" s="5"/>
       <c r="W26" s="5"/>
       <c r="X26" s="7">
-        <v>0.33</v>
-      </c>
-      <c r="Y26" s="9">
-        <v>1</v>
-      </c>
-      <c r="Z26" s="9">
-        <v>0</v>
-      </c>
-      <c r="AA26" s="9">
+        <f>COUNTIF(X23:X25,"Y")/3</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="Y26" s="7">
+        <f t="shared" ref="Y26:AA26" si="8">COUNTIF(Y23:Y25,"Y")/3</f>
+        <v>1</v>
+      </c>
+      <c r="Z26" s="7">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AA26" s="7">
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="V27" s="2" t="s">
+      <c r="V27" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="W27" s="2"/>
-      <c r="X27" s="6">
-        <v>8.3000000000000004E-2</v>
-      </c>
-      <c r="Y27" s="8">
-        <v>0.91700000000000004</v>
-      </c>
-      <c r="Z27" s="8">
-        <v>0</v>
-      </c>
-      <c r="AA27" s="8">
+      <c r="W27" s="13"/>
+      <c r="X27" s="14">
+        <f>AVERAGE(X11:X26)</f>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="Y27" s="14">
+        <f t="shared" ref="Y27:AA27" si="9">AVERAGE(Y11:Y26)</f>
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="Z27" s="14">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AA27" s="14">
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -7900,29 +8106,37 @@
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
       <c r="F35" s="7">
-        <v>1</v>
-      </c>
-      <c r="G35" s="9">
-        <v>0.67</v>
-      </c>
-      <c r="H35" s="9">
-        <v>0</v>
-      </c>
-      <c r="I35" s="9">
-        <v>0</v>
-      </c>
-      <c r="J35" s="9">
-        <v>1</v>
-      </c>
-      <c r="K35" s="9"/>
-      <c r="L35" s="9">
-        <v>0.67</v>
-      </c>
-      <c r="M35" s="9">
-        <v>0.67</v>
-      </c>
-      <c r="N35" s="9">
-        <v>0.67</v>
+        <f>COUNTIF(F32:F34,"Y")/3</f>
+        <v>1</v>
+      </c>
+      <c r="G35" s="7">
+        <f t="shared" ref="G35:N35" si="10">COUNTIF(G32:G34,"Y")/3</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="H35" s="7">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="I35" s="7">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="J35" s="7">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="K35" s="7"/>
+      <c r="L35" s="7">
+        <f t="shared" si="10"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="M35" s="7">
+        <f t="shared" si="10"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="N35" s="7">
+        <f t="shared" si="10"/>
+        <v>0.66666666666666663</v>
       </c>
       <c r="W35">
         <v>2</v>
@@ -7975,15 +8189,19 @@
       <c r="V36" s="2"/>
       <c r="W36" s="2"/>
       <c r="X36" s="7">
-        <v>0.33</v>
-      </c>
-      <c r="Y36" s="9">
-        <v>1</v>
-      </c>
-      <c r="Z36" s="9">
-        <v>0.33</v>
-      </c>
-      <c r="AA36" s="9">
+        <f>COUNTIF(X33:X35,"Y")/3</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="Y36" s="7">
+        <f t="shared" ref="Y36:AA36" si="11">COUNTIF(Y33:Y35,"Y")/3</f>
+        <v>1</v>
+      </c>
+      <c r="Z36" s="7">
+        <f t="shared" si="11"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="AA36" s="7">
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -8084,29 +8302,37 @@
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
       <c r="F39" s="7">
-        <v>1</v>
-      </c>
-      <c r="G39" s="9">
-        <v>1</v>
-      </c>
-      <c r="H39" s="9">
-        <v>0</v>
-      </c>
-      <c r="I39" s="9">
-        <v>0.33</v>
-      </c>
-      <c r="J39" s="9">
-        <v>1</v>
-      </c>
-      <c r="K39" s="9"/>
-      <c r="L39" s="9">
-        <v>0.67</v>
-      </c>
-      <c r="M39" s="9">
-        <v>0</v>
-      </c>
-      <c r="N39" s="9">
-        <v>0.33</v>
+        <f>COUNTIF(F36:F38,"Y")/3</f>
+        <v>1</v>
+      </c>
+      <c r="G39" s="7">
+        <f t="shared" ref="G39:N39" si="12">COUNTIF(G36:G38,"Y")/3</f>
+        <v>1</v>
+      </c>
+      <c r="H39" s="7">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="I39" s="7">
+        <f t="shared" si="12"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="J39" s="7">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="K39" s="7"/>
+      <c r="L39" s="7">
+        <f t="shared" si="12"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="M39" s="7">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="N39" s="7">
+        <f t="shared" si="12"/>
+        <v>0.33333333333333331</v>
       </c>
       <c r="W39">
         <v>2</v>
@@ -8159,15 +8385,19 @@
       <c r="V40" s="2"/>
       <c r="W40" s="2"/>
       <c r="X40" s="7">
-        <v>0.67</v>
-      </c>
-      <c r="Y40" s="9">
-        <v>1</v>
-      </c>
-      <c r="Z40" s="9">
-        <v>0.67</v>
-      </c>
-      <c r="AA40" s="9">
+        <f>COUNTIF(X37:X39,"Y")/3</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="Y40" s="7">
+        <f t="shared" ref="Y40:AA40" si="13">COUNTIF(Y37:Y39,"Y")/3</f>
+        <v>1</v>
+      </c>
+      <c r="Z40" s="7">
+        <f t="shared" si="13"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="AA40" s="7">
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
     </row>
@@ -8268,28 +8498,36 @@
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
       <c r="F43" s="7">
-        <v>1</v>
-      </c>
-      <c r="G43" s="9">
-        <v>1</v>
-      </c>
-      <c r="H43" s="9">
-        <v>0.33</v>
-      </c>
-      <c r="I43" s="9">
-        <v>0.67</v>
-      </c>
-      <c r="J43" s="9">
-        <v>1</v>
-      </c>
-      <c r="K43" s="9"/>
-      <c r="L43" s="9">
-        <v>0</v>
-      </c>
-      <c r="M43" s="9">
-        <v>0</v>
-      </c>
-      <c r="N43" s="9">
+        <f>COUNTIF(F40:F42,"Y")/3</f>
+        <v>1</v>
+      </c>
+      <c r="G43" s="7">
+        <f t="shared" ref="G43:N43" si="14">COUNTIF(G40:G42,"Y")/3</f>
+        <v>1</v>
+      </c>
+      <c r="H43" s="7">
+        <f t="shared" si="14"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I43" s="7">
+        <f t="shared" si="14"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="J43" s="7">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="K43" s="7"/>
+      <c r="L43" s="7">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="M43" s="7">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="N43" s="7">
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="W43">
@@ -8343,15 +8581,19 @@
       <c r="V44" s="2"/>
       <c r="W44" s="2"/>
       <c r="X44" s="7">
-        <v>0.33</v>
-      </c>
-      <c r="Y44" s="9">
-        <v>1</v>
-      </c>
-      <c r="Z44" s="9">
-        <v>0.33</v>
-      </c>
-      <c r="AA44" s="9">
+        <f>COUNTIF(X41:X43,"Y")/3</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="Y44" s="7">
+        <f t="shared" ref="Y44:AA44" si="15">COUNTIF(Y41:Y43,"Y")/3</f>
+        <v>1</v>
+      </c>
+      <c r="Z44" s="7">
+        <f t="shared" si="15"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="AA44" s="7">
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -8452,28 +8694,36 @@
       <c r="D47" s="5"/>
       <c r="E47" s="5"/>
       <c r="F47" s="7">
-        <v>1</v>
-      </c>
-      <c r="G47" s="9">
-        <v>1</v>
-      </c>
-      <c r="H47" s="9">
-        <v>0.33</v>
-      </c>
-      <c r="I47" s="9">
-        <v>0</v>
-      </c>
-      <c r="J47" s="9">
-        <v>1</v>
-      </c>
-      <c r="K47" s="9"/>
-      <c r="L47" s="9">
-        <v>0.67</v>
-      </c>
-      <c r="M47" s="9">
-        <v>0.33</v>
-      </c>
-      <c r="N47" s="9">
+        <f>COUNTIF(F44:F46,"Y")/3</f>
+        <v>1</v>
+      </c>
+      <c r="G47" s="7">
+        <f t="shared" ref="G47:N47" si="16">COUNTIF(G44:G46,"Y")/3</f>
+        <v>1</v>
+      </c>
+      <c r="H47" s="7">
+        <f t="shared" si="16"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I47" s="7">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="J47" s="7">
+        <f t="shared" si="16"/>
+        <v>1</v>
+      </c>
+      <c r="K47" s="7"/>
+      <c r="L47" s="7">
+        <f t="shared" si="16"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="M47" s="7">
+        <f t="shared" si="16"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="N47" s="7">
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="W47">
@@ -8498,60 +8748,76 @@
       </c>
       <c r="E48" s="2"/>
       <c r="F48" s="6">
-        <v>1</v>
-      </c>
-      <c r="G48" s="8">
-        <v>0.91700000000000004</v>
-      </c>
-      <c r="H48" s="8">
-        <v>0.16700000000000001</v>
-      </c>
-      <c r="I48" s="8">
+        <f>AVERAGE(F32:F47)</f>
+        <v>1</v>
+      </c>
+      <c r="G48" s="6">
+        <f t="shared" ref="G48:N48" si="17">AVERAGE(G32:G47)</f>
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="H48" s="6">
+        <f t="shared" si="17"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="I48" s="6">
+        <f t="shared" si="17"/>
         <v>0.25</v>
       </c>
-      <c r="J48" s="8">
-        <v>1</v>
-      </c>
-      <c r="K48" s="8"/>
-      <c r="L48" s="8">
+      <c r="J48" s="6">
+        <f t="shared" si="17"/>
+        <v>1</v>
+      </c>
+      <c r="K48" s="6"/>
+      <c r="L48" s="6">
+        <f t="shared" si="17"/>
         <v>0.5</v>
       </c>
-      <c r="M48" s="8">
+      <c r="M48" s="6">
+        <f t="shared" si="17"/>
         <v>0.25</v>
       </c>
-      <c r="N48" s="8">
+      <c r="N48" s="6">
+        <f t="shared" si="17"/>
         <v>0.25</v>
       </c>
       <c r="V48" s="5"/>
       <c r="W48" s="5"/>
       <c r="X48" s="7">
-        <v>0.33</v>
-      </c>
-      <c r="Y48" s="9">
-        <v>1</v>
-      </c>
-      <c r="Z48" s="9">
-        <v>0.33</v>
-      </c>
-      <c r="AA48" s="9">
+        <f>COUNTIF(X45:X47,"Y")/3</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="Y48" s="7">
+        <f t="shared" ref="Y48:AA48" si="18">COUNTIF(Y45:Y47,"Y")/3</f>
+        <v>1</v>
+      </c>
+      <c r="Z48" s="7">
+        <f t="shared" si="18"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="AA48" s="7">
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
     </row>
     <row r="49" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="V49" s="2" t="s">
+      <c r="V49" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="W49" s="2"/>
-      <c r="X49" s="6">
-        <v>0.41699999999999998</v>
-      </c>
-      <c r="Y49" s="8">
-        <v>1</v>
-      </c>
-      <c r="Z49" s="8">
-        <v>0.41699999999999998</v>
-      </c>
-      <c r="AA49" s="8">
+      <c r="W49" s="13"/>
+      <c r="X49" s="14">
+        <f>AVERAGE(X33:X48)</f>
+        <v>0.41666666666666663</v>
+      </c>
+      <c r="Y49" s="14">
+        <f t="shared" ref="Y49:AA49" si="19">AVERAGE(Y33:Y48)</f>
+        <v>1</v>
+      </c>
+      <c r="Z49" s="14">
+        <f t="shared" si="19"/>
+        <v>0.41666666666666663</v>
+      </c>
+      <c r="AA49" s="14">
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -8745,28 +9011,36 @@
       <c r="D56" s="2"/>
       <c r="E56" s="2"/>
       <c r="F56" s="7">
-        <v>1</v>
-      </c>
-      <c r="G56" s="9">
-        <v>1</v>
-      </c>
-      <c r="H56" s="9">
-        <v>0</v>
-      </c>
-      <c r="I56" s="9">
-        <v>0</v>
-      </c>
-      <c r="J56" s="9">
-        <v>0</v>
-      </c>
-      <c r="K56" s="9"/>
-      <c r="L56" s="9">
-        <v>1</v>
-      </c>
-      <c r="M56" s="9">
-        <v>1</v>
-      </c>
-      <c r="N56" s="9">
+        <f>COUNTIF(F53:F55,"Y")/3</f>
+        <v>1</v>
+      </c>
+      <c r="G56" s="7">
+        <f t="shared" ref="G56:N56" si="20">COUNTIF(G53:G55,"Y")/3</f>
+        <v>1</v>
+      </c>
+      <c r="H56" s="7">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="I56" s="7">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="J56" s="7">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="K56" s="7"/>
+      <c r="L56" s="7">
+        <f t="shared" si="20"/>
+        <v>1</v>
+      </c>
+      <c r="M56" s="7">
+        <f t="shared" si="20"/>
+        <v>1</v>
+      </c>
+      <c r="N56" s="7">
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="W56">
@@ -8865,15 +9139,19 @@
       <c r="V58" s="2"/>
       <c r="W58" s="2"/>
       <c r="X58" s="7">
-        <v>0</v>
-      </c>
-      <c r="Y58" s="9">
-        <v>1</v>
-      </c>
-      <c r="Z58" s="9">
-        <v>0</v>
-      </c>
-      <c r="AA58" s="9">
+        <f>COUNTIF(X55:X57,"Y")/3</f>
+        <v>0</v>
+      </c>
+      <c r="Y58" s="7">
+        <f t="shared" ref="Y58:AA58" si="21">COUNTIF(Y55:Y57,"Y")/3</f>
+        <v>1</v>
+      </c>
+      <c r="Z58" s="7">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="AA58" s="7">
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -8929,29 +9207,37 @@
       <c r="D60" s="2"/>
       <c r="E60" s="2"/>
       <c r="F60" s="7">
-        <v>1</v>
-      </c>
-      <c r="G60" s="9">
-        <v>1</v>
-      </c>
-      <c r="H60" s="9">
-        <v>0.33</v>
-      </c>
-      <c r="I60" s="9">
-        <v>0</v>
-      </c>
-      <c r="J60" s="9">
-        <v>0</v>
-      </c>
-      <c r="K60" s="9"/>
-      <c r="L60" s="9">
-        <v>0.33</v>
-      </c>
-      <c r="M60" s="9">
-        <v>0.67</v>
-      </c>
-      <c r="N60" s="9">
-        <v>0.33</v>
+        <f>COUNTIF(F57:F59,"Y")/3</f>
+        <v>1</v>
+      </c>
+      <c r="G60" s="7">
+        <f t="shared" ref="G60:N60" si="22">COUNTIF(G57:G59,"Y")/3</f>
+        <v>1</v>
+      </c>
+      <c r="H60" s="7">
+        <f t="shared" si="22"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I60" s="7">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="J60" s="7">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="K60" s="7"/>
+      <c r="L60" s="7">
+        <f t="shared" si="22"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="M60" s="7">
+        <f t="shared" si="22"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="N60" s="7">
+        <f t="shared" si="22"/>
+        <v>0.33333333333333331</v>
       </c>
       <c r="W60">
         <v>1</v>
@@ -9049,15 +9335,19 @@
       <c r="V62" s="2"/>
       <c r="W62" s="2"/>
       <c r="X62" s="7">
-        <v>0.33</v>
-      </c>
-      <c r="Y62" s="9">
-        <v>1</v>
-      </c>
-      <c r="Z62" s="9">
-        <v>0.33</v>
-      </c>
-      <c r="AA62" s="9">
+        <f>COUNTIF(X59:X61,"Y")/3</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="Y62" s="7">
+        <f t="shared" ref="Y62:AA62" si="23">COUNTIF(Y59:Y61,"Y")/3</f>
+        <v>1</v>
+      </c>
+      <c r="Z62" s="7">
+        <f t="shared" si="23"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="AA62" s="7">
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
     </row>
@@ -9113,28 +9403,36 @@
       <c r="D64" s="2"/>
       <c r="E64" s="2"/>
       <c r="F64" s="7">
-        <v>1</v>
-      </c>
-      <c r="G64" s="9">
-        <v>1</v>
-      </c>
-      <c r="H64" s="9">
-        <v>1</v>
-      </c>
-      <c r="I64" s="9">
-        <v>0</v>
-      </c>
-      <c r="J64" s="9">
-        <v>0.33</v>
-      </c>
-      <c r="K64" s="9"/>
-      <c r="L64" s="9">
-        <v>1</v>
-      </c>
-      <c r="M64" s="9">
-        <v>1</v>
-      </c>
-      <c r="N64" s="9">
+        <f>COUNTIF(F61:F63,"Y")/3</f>
+        <v>1</v>
+      </c>
+      <c r="G64" s="7">
+        <f t="shared" ref="G64:N64" si="24">COUNTIF(G61:G63,"Y")/3</f>
+        <v>1</v>
+      </c>
+      <c r="H64" s="7">
+        <f t="shared" si="24"/>
+        <v>1</v>
+      </c>
+      <c r="I64" s="7">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="J64" s="7">
+        <f t="shared" si="24"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="K64" s="7"/>
+      <c r="L64" s="7">
+        <f t="shared" si="24"/>
+        <v>1</v>
+      </c>
+      <c r="M64" s="7">
+        <f t="shared" si="24"/>
+        <v>1</v>
+      </c>
+      <c r="N64" s="7">
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="W64">
@@ -9233,15 +9531,19 @@
       <c r="V66" s="2"/>
       <c r="W66" s="2"/>
       <c r="X66" s="7">
-        <v>1</v>
-      </c>
-      <c r="Y66" s="9">
-        <v>1</v>
-      </c>
-      <c r="Z66" s="9">
-        <v>1</v>
-      </c>
-      <c r="AA66" s="9">
+        <f>COUNTIF(X63:X65,"Y")/3</f>
+        <v>1</v>
+      </c>
+      <c r="Y66" s="7">
+        <f t="shared" ref="Y66:AA66" si="25">COUNTIF(Y63:Y65,"Y")/3</f>
+        <v>1</v>
+      </c>
+      <c r="Z66" s="7">
+        <f t="shared" si="25"/>
+        <v>1</v>
+      </c>
+      <c r="AA66" s="7">
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
     </row>
@@ -9297,29 +9599,37 @@
       <c r="D68" s="5"/>
       <c r="E68" s="5"/>
       <c r="F68" s="7">
-        <v>1</v>
-      </c>
-      <c r="G68" s="9">
-        <v>1</v>
-      </c>
-      <c r="H68" s="9">
-        <v>1</v>
-      </c>
-      <c r="I68" s="9">
-        <v>0</v>
-      </c>
-      <c r="J68" s="9">
-        <v>0.33</v>
-      </c>
-      <c r="K68" s="9"/>
-      <c r="L68" s="9">
-        <v>0.33</v>
-      </c>
-      <c r="M68" s="9">
-        <v>0.33</v>
-      </c>
-      <c r="N68" s="9">
-        <v>0.33</v>
+        <f>COUNTIF(F65:F67,"Y")/3</f>
+        <v>1</v>
+      </c>
+      <c r="G68" s="7">
+        <f t="shared" ref="G68:N68" si="26">COUNTIF(G65:G67,"Y")/3</f>
+        <v>1</v>
+      </c>
+      <c r="H68" s="7">
+        <f t="shared" si="26"/>
+        <v>1</v>
+      </c>
+      <c r="I68" s="7">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+      <c r="J68" s="7">
+        <f t="shared" si="26"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="K68" s="7"/>
+      <c r="L68" s="7">
+        <f t="shared" si="26"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="M68" s="7">
+        <f t="shared" si="26"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="N68" s="7">
+        <f t="shared" si="26"/>
+        <v>0.33333333333333331</v>
       </c>
       <c r="W68">
         <v>1</v>
@@ -9343,29 +9653,37 @@
       </c>
       <c r="E69" s="2"/>
       <c r="F69" s="6">
-        <v>1</v>
-      </c>
-      <c r="G69" s="8">
-        <v>1</v>
-      </c>
-      <c r="H69" s="8">
-        <v>0.58299999999999996</v>
-      </c>
-      <c r="I69" s="8">
-        <v>0</v>
-      </c>
-      <c r="J69" s="8">
-        <v>0.16700000000000001</v>
-      </c>
-      <c r="K69" s="8"/>
-      <c r="L69" s="8">
-        <v>0.66700000000000004</v>
-      </c>
-      <c r="M69" s="8">
+        <f>AVERAGE(F53:F68)</f>
+        <v>1</v>
+      </c>
+      <c r="G69" s="6">
+        <f t="shared" ref="G69:N69" si="27">AVERAGE(G53:G68)</f>
+        <v>1</v>
+      </c>
+      <c r="H69" s="6">
+        <f t="shared" si="27"/>
+        <v>0.58333333333333326</v>
+      </c>
+      <c r="I69" s="6">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+      <c r="J69" s="6">
+        <f t="shared" si="27"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="K69" s="6"/>
+      <c r="L69" s="6">
+        <f t="shared" si="27"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="M69" s="6">
+        <f t="shared" si="27"/>
         <v>0.75</v>
       </c>
-      <c r="N69" s="8">
-        <v>0.16700000000000001</v>
+      <c r="N69" s="6">
+        <f t="shared" si="27"/>
+        <v>0.16666666666666666</v>
       </c>
       <c r="W69">
         <v>2</v>
@@ -9387,33 +9705,41 @@
       <c r="V70" s="5"/>
       <c r="W70" s="5"/>
       <c r="X70" s="7">
-        <v>1</v>
-      </c>
-      <c r="Y70" s="9">
-        <v>1</v>
-      </c>
-      <c r="Z70" s="9">
-        <v>1</v>
-      </c>
-      <c r="AA70" s="9">
+        <f>COUNTIF(X67:X69,"Y")/3</f>
+        <v>1</v>
+      </c>
+      <c r="Y70" s="7">
+        <f t="shared" ref="Y70:Z70" si="28">COUNTIF(Y67:Y69,"Y")/3</f>
+        <v>1</v>
+      </c>
+      <c r="Z70" s="7">
+        <f t="shared" si="28"/>
+        <v>1</v>
+      </c>
+      <c r="AA70" s="7">
+        <f t="shared" ref="AA70" si="29">COUNTIF(AA67:AA69,"Y")/3</f>
         <v>0</v>
       </c>
     </row>
     <row r="71" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="V71" s="2" t="s">
+      <c r="V71" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="W71" s="2"/>
-      <c r="X71" s="6">
-        <v>0.58299999999999996</v>
-      </c>
-      <c r="Y71" s="8">
-        <v>1</v>
-      </c>
-      <c r="Z71" s="8">
-        <v>0.58299999999999996</v>
-      </c>
-      <c r="AA71" s="8">
+      <c r="W71" s="13"/>
+      <c r="X71" s="14">
+        <f>AVERAGE(X55:X70)</f>
+        <v>0.58333333333333326</v>
+      </c>
+      <c r="Y71" s="14">
+        <f t="shared" ref="Y71:AA71" si="30">AVERAGE(Y55:Y70)</f>
+        <v>1</v>
+      </c>
+      <c r="Z71" s="14">
+        <f t="shared" si="30"/>
+        <v>0.58333333333333326</v>
+      </c>
+      <c r="AA71" s="14">
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
     </row>
@@ -9589,28 +9915,36 @@
       <c r="D77" s="2"/>
       <c r="E77" s="2"/>
       <c r="F77" s="7">
-        <v>1</v>
-      </c>
-      <c r="G77" s="9">
-        <v>1</v>
-      </c>
-      <c r="H77" s="9">
-        <v>1</v>
-      </c>
-      <c r="I77" s="9">
-        <v>0</v>
-      </c>
-      <c r="J77" s="9">
-        <v>1</v>
-      </c>
-      <c r="K77" s="9"/>
-      <c r="L77" s="9">
-        <v>1</v>
-      </c>
-      <c r="M77" s="9">
-        <v>0.33</v>
-      </c>
-      <c r="N77" s="9">
+        <f>COUNTIF(F74:F76,"Y")/3</f>
+        <v>1</v>
+      </c>
+      <c r="G77" s="7">
+        <f t="shared" ref="G77:N77" si="31">COUNTIF(G74:G76,"Y")/3</f>
+        <v>1</v>
+      </c>
+      <c r="H77" s="7">
+        <f t="shared" si="31"/>
+        <v>1</v>
+      </c>
+      <c r="I77" s="7">
+        <f t="shared" si="31"/>
+        <v>0</v>
+      </c>
+      <c r="J77" s="7">
+        <f t="shared" si="31"/>
+        <v>1</v>
+      </c>
+      <c r="K77" s="7"/>
+      <c r="L77" s="7">
+        <f t="shared" si="31"/>
+        <v>1</v>
+      </c>
+      <c r="M77" s="7">
+        <f t="shared" si="31"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="N77" s="7">
+        <f t="shared" si="31"/>
         <v>1</v>
       </c>
       <c r="V77">
@@ -9757,15 +10091,19 @@
       <c r="V80" s="2"/>
       <c r="W80" s="2"/>
       <c r="X80" s="7">
-        <v>1</v>
-      </c>
-      <c r="Y80" s="9">
-        <v>1</v>
-      </c>
-      <c r="Z80" s="9">
-        <v>1</v>
-      </c>
-      <c r="AA80" s="9">
+        <f>COUNTIF(X77:X79,"Y")/3</f>
+        <v>1</v>
+      </c>
+      <c r="Y80" s="7">
+        <f t="shared" ref="Y80:AA80" si="32">COUNTIF(Y77:Y79,"Y")/3</f>
+        <v>1</v>
+      </c>
+      <c r="Z80" s="7">
+        <f t="shared" si="32"/>
+        <v>1</v>
+      </c>
+      <c r="AA80" s="7">
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
     </row>
@@ -9773,28 +10111,36 @@
       <c r="D81" s="2"/>
       <c r="E81" s="2"/>
       <c r="F81" s="7">
-        <v>1</v>
-      </c>
-      <c r="G81" s="9">
-        <v>1</v>
-      </c>
-      <c r="H81" s="9">
-        <v>1</v>
-      </c>
-      <c r="I81" s="9">
-        <v>0</v>
-      </c>
-      <c r="J81" s="9">
-        <v>1</v>
-      </c>
-      <c r="K81" s="9"/>
-      <c r="L81" s="9">
-        <v>1</v>
-      </c>
-      <c r="M81" s="9">
-        <v>0.33</v>
-      </c>
-      <c r="N81" s="9">
+        <f>COUNTIF(F78:F80,"Y")/3</f>
+        <v>1</v>
+      </c>
+      <c r="G81" s="7">
+        <f t="shared" ref="G81:N81" si="33">COUNTIF(G78:G80,"Y")/3</f>
+        <v>1</v>
+      </c>
+      <c r="H81" s="7">
+        <f t="shared" si="33"/>
+        <v>1</v>
+      </c>
+      <c r="I81" s="7">
+        <f t="shared" si="33"/>
+        <v>0</v>
+      </c>
+      <c r="J81" s="7">
+        <f t="shared" si="33"/>
+        <v>1</v>
+      </c>
+      <c r="K81" s="7"/>
+      <c r="L81" s="7">
+        <f t="shared" si="33"/>
+        <v>1</v>
+      </c>
+      <c r="M81" s="7">
+        <f t="shared" si="33"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="N81" s="7">
+        <f t="shared" si="33"/>
         <v>1</v>
       </c>
       <c r="V81">
@@ -9941,15 +10287,19 @@
       <c r="V84" s="2"/>
       <c r="W84" s="2"/>
       <c r="X84" s="7">
-        <v>1</v>
-      </c>
-      <c r="Y84" s="9">
-        <v>1</v>
-      </c>
-      <c r="Z84" s="9">
-        <v>1</v>
-      </c>
-      <c r="AA84" s="9">
+        <f>COUNTIF(X81:X83,"Y")/3</f>
+        <v>1</v>
+      </c>
+      <c r="Y84" s="7">
+        <f t="shared" ref="Y84:AA84" si="34">COUNTIF(Y81:Y83,"Y")/3</f>
+        <v>1</v>
+      </c>
+      <c r="Z84" s="7">
+        <f t="shared" si="34"/>
+        <v>1</v>
+      </c>
+      <c r="AA84" s="7">
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
     </row>
@@ -9957,29 +10307,37 @@
       <c r="D85" s="2"/>
       <c r="E85" s="2"/>
       <c r="F85" s="7">
-        <v>1</v>
-      </c>
-      <c r="G85" s="9">
-        <v>1</v>
-      </c>
-      <c r="H85" s="9">
-        <v>1</v>
-      </c>
-      <c r="I85" s="9">
-        <v>0.33</v>
-      </c>
-      <c r="J85" s="9">
-        <v>1</v>
-      </c>
-      <c r="K85" s="9"/>
-      <c r="L85" s="9">
-        <v>0</v>
-      </c>
-      <c r="M85" s="9">
-        <v>0.67</v>
-      </c>
-      <c r="N85" s="9">
-        <v>0.67</v>
+        <f>COUNTIF(F82:F84,"Y")/3</f>
+        <v>1</v>
+      </c>
+      <c r="G85" s="7">
+        <f t="shared" ref="G85:N85" si="35">COUNTIF(G82:G84,"Y")/3</f>
+        <v>1</v>
+      </c>
+      <c r="H85" s="7">
+        <f t="shared" si="35"/>
+        <v>1</v>
+      </c>
+      <c r="I85" s="7">
+        <f t="shared" si="35"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="J85" s="7">
+        <f t="shared" si="35"/>
+        <v>1</v>
+      </c>
+      <c r="K85" s="7"/>
+      <c r="L85" s="7">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="M85" s="7">
+        <f t="shared" si="35"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="N85" s="7">
+        <f t="shared" si="35"/>
+        <v>0.66666666666666663</v>
       </c>
       <c r="V85">
         <v>0.7</v>
@@ -10125,45 +10483,57 @@
       <c r="V88" s="2"/>
       <c r="W88" s="2"/>
       <c r="X88" s="7">
-        <v>1</v>
-      </c>
-      <c r="Y88" s="9">
-        <v>1</v>
-      </c>
-      <c r="Z88" s="9">
-        <v>1</v>
-      </c>
-      <c r="AA88" s="9">
-        <v>0.33</v>
+        <f>COUNTIF(X85:X87,"Y")/3</f>
+        <v>1</v>
+      </c>
+      <c r="Y88" s="7">
+        <f t="shared" ref="Y88:AA88" si="36">COUNTIF(Y85:Y87,"Y")/3</f>
+        <v>1</v>
+      </c>
+      <c r="Z88" s="7">
+        <f t="shared" si="36"/>
+        <v>1</v>
+      </c>
+      <c r="AA88" s="7">
+        <f t="shared" si="36"/>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="89" spans="2:27" x14ac:dyDescent="0.3">
       <c r="D89" s="5"/>
       <c r="E89" s="5"/>
       <c r="F89" s="7">
-        <v>1</v>
-      </c>
-      <c r="G89" s="9">
-        <v>1</v>
-      </c>
-      <c r="H89" s="9">
-        <v>1</v>
-      </c>
-      <c r="I89" s="9">
-        <v>0.67</v>
-      </c>
-      <c r="J89" s="9">
-        <v>1</v>
-      </c>
-      <c r="K89" s="9"/>
-      <c r="L89" s="9">
-        <v>0.67</v>
-      </c>
-      <c r="M89" s="9">
-        <v>0.33</v>
-      </c>
-      <c r="N89" s="9">
-        <v>0.67</v>
+        <f>COUNTIF(F86:F88,"Y")/3</f>
+        <v>1</v>
+      </c>
+      <c r="G89" s="7">
+        <f t="shared" ref="G89:N89" si="37">COUNTIF(G86:G88,"Y")/3</f>
+        <v>1</v>
+      </c>
+      <c r="H89" s="7">
+        <f t="shared" si="37"/>
+        <v>1</v>
+      </c>
+      <c r="I89" s="7">
+        <f t="shared" si="37"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="J89" s="7">
+        <f t="shared" si="37"/>
+        <v>1</v>
+      </c>
+      <c r="K89" s="7"/>
+      <c r="L89" s="7">
+        <f t="shared" si="37"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="M89" s="7">
+        <f t="shared" si="37"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="N89" s="7">
+        <f t="shared" si="37"/>
+        <v>0.66666666666666663</v>
       </c>
       <c r="V89">
         <v>1</v>
@@ -10190,29 +10560,37 @@
       </c>
       <c r="E90" s="2"/>
       <c r="F90" s="6">
-        <v>1</v>
-      </c>
-      <c r="G90" s="8">
-        <v>1</v>
-      </c>
-      <c r="H90" s="8">
-        <v>1</v>
-      </c>
-      <c r="I90" s="8">
-        <v>0.25</v>
-      </c>
-      <c r="J90" s="8">
-        <v>1</v>
-      </c>
-      <c r="K90" s="8"/>
-      <c r="L90" s="8">
-        <v>0.66700000000000004</v>
-      </c>
-      <c r="M90" s="8">
-        <v>0.41699999999999998</v>
-      </c>
-      <c r="N90" s="8">
-        <v>0.83299999999999996</v>
+        <f>AVERAGE(F74:F88)</f>
+        <v>1</v>
+      </c>
+      <c r="G90" s="6">
+        <f t="shared" ref="G90:N90" si="38">AVERAGE(G74:G88)</f>
+        <v>1</v>
+      </c>
+      <c r="H90" s="6">
+        <f t="shared" si="38"/>
+        <v>1</v>
+      </c>
+      <c r="I90" s="6">
+        <f t="shared" si="38"/>
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="J90" s="6">
+        <f t="shared" si="38"/>
+        <v>1</v>
+      </c>
+      <c r="K90" s="6"/>
+      <c r="L90" s="6">
+        <f t="shared" si="38"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="M90" s="6">
+        <f t="shared" si="38"/>
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="N90" s="6">
+        <f t="shared" si="38"/>
+        <v>0.88888888888888884</v>
       </c>
       <c r="W90">
         <v>1</v>
@@ -10281,16 +10659,20 @@
       <c r="V92" s="5"/>
       <c r="W92" s="5"/>
       <c r="X92" s="7">
-        <v>1</v>
-      </c>
-      <c r="Y92" s="9">
-        <v>1</v>
-      </c>
-      <c r="Z92" s="9">
-        <v>1</v>
-      </c>
-      <c r="AA92" s="9">
-        <v>0.33</v>
+        <f>COUNTIF(X89:X91,"Y")/3</f>
+        <v>1</v>
+      </c>
+      <c r="Y92" s="7">
+        <f t="shared" ref="Y92:AA92" si="39">COUNTIF(Y89:Y91,"Y")/3</f>
+        <v>1</v>
+      </c>
+      <c r="Z92" s="7">
+        <f t="shared" si="39"/>
+        <v>1</v>
+      </c>
+      <c r="AA92" s="7">
+        <f t="shared" si="39"/>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="93" spans="2:27" x14ac:dyDescent="0.3">
@@ -10308,21 +10690,25 @@
       <c r="L93" s="2"/>
       <c r="M93" s="2"/>
       <c r="N93" s="2"/>
-      <c r="V93" s="2" t="s">
+      <c r="V93" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="W93" s="2"/>
-      <c r="X93" s="6">
-        <v>1</v>
-      </c>
-      <c r="Y93" s="8">
-        <v>1</v>
-      </c>
-      <c r="Z93" s="8">
-        <v>1</v>
-      </c>
-      <c r="AA93" s="8">
-        <v>0.16700000000000001</v>
+      <c r="W93" s="13"/>
+      <c r="X93" s="14">
+        <f>AVERAGE(X77:X92)</f>
+        <v>1</v>
+      </c>
+      <c r="Y93" s="14">
+        <f t="shared" ref="Y93:AA93" si="40">AVERAGE(Y77:Y92)</f>
+        <v>1</v>
+      </c>
+      <c r="Z93" s="14">
+        <f t="shared" si="40"/>
+        <v>1</v>
+      </c>
+      <c r="AA93" s="14">
+        <f t="shared" si="40"/>
+        <v>0.16666666666666666</v>
       </c>
     </row>
     <row r="94" spans="2:27" x14ac:dyDescent="0.3">
@@ -10422,28 +10808,36 @@
       <c r="D97" s="2"/>
       <c r="E97" s="2"/>
       <c r="F97" s="7">
-        <v>1</v>
-      </c>
-      <c r="G97" s="9">
-        <v>1</v>
-      </c>
-      <c r="H97" s="9">
-        <v>1</v>
-      </c>
-      <c r="I97" s="9">
-        <v>0</v>
-      </c>
-      <c r="J97" s="9">
-        <v>0</v>
-      </c>
-      <c r="K97" s="9"/>
-      <c r="L97" s="9">
-        <v>0.33</v>
-      </c>
-      <c r="M97" s="9">
-        <v>1</v>
-      </c>
-      <c r="N97" s="9">
+        <f>COUNTIF(F94:F96,"Y")/3</f>
+        <v>1</v>
+      </c>
+      <c r="G97" s="7">
+        <f t="shared" ref="G97:N97" si="41">COUNTIF(G94:G96,"Y")/3</f>
+        <v>1</v>
+      </c>
+      <c r="H97" s="7">
+        <f t="shared" si="41"/>
+        <v>1</v>
+      </c>
+      <c r="I97" s="7">
+        <f t="shared" si="41"/>
+        <v>0</v>
+      </c>
+      <c r="J97" s="7">
+        <f t="shared" si="41"/>
+        <v>0</v>
+      </c>
+      <c r="K97" s="7"/>
+      <c r="L97" s="7">
+        <f t="shared" si="41"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="M97" s="7">
+        <f t="shared" si="41"/>
+        <v>1</v>
+      </c>
+      <c r="N97" s="7">
+        <f t="shared" si="41"/>
         <v>1</v>
       </c>
     </row>
@@ -10589,29 +10983,37 @@
       <c r="D101" s="2"/>
       <c r="E101" s="2"/>
       <c r="F101" s="7">
-        <v>1</v>
-      </c>
-      <c r="G101" s="9">
-        <v>1</v>
-      </c>
-      <c r="H101" s="9">
-        <v>1</v>
-      </c>
-      <c r="I101" s="9">
-        <v>0.67</v>
-      </c>
-      <c r="J101" s="9">
-        <v>0.33</v>
-      </c>
-      <c r="K101" s="9"/>
-      <c r="L101" s="9">
-        <v>0</v>
-      </c>
-      <c r="M101" s="9">
-        <v>1</v>
-      </c>
-      <c r="N101" s="9">
-        <v>0.67</v>
+        <f>COUNTIF(F98:F100,"Y")/3</f>
+        <v>1</v>
+      </c>
+      <c r="G101" s="7">
+        <f t="shared" ref="G101:N101" si="42">COUNTIF(G98:G100,"Y")/3</f>
+        <v>1</v>
+      </c>
+      <c r="H101" s="7">
+        <f t="shared" si="42"/>
+        <v>1</v>
+      </c>
+      <c r="I101" s="7">
+        <f t="shared" si="42"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="J101" s="7">
+        <f t="shared" si="42"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="K101" s="7"/>
+      <c r="L101" s="7">
+        <f t="shared" si="42"/>
+        <v>0</v>
+      </c>
+      <c r="M101" s="7">
+        <f t="shared" si="42"/>
+        <v>1</v>
+      </c>
+      <c r="N101" s="7">
+        <f t="shared" si="42"/>
+        <v>0.66666666666666663</v>
       </c>
       <c r="W101">
         <v>1</v>
@@ -10709,15 +11111,19 @@
       <c r="V103" s="2"/>
       <c r="W103" s="2"/>
       <c r="X103" s="7">
-        <v>1</v>
-      </c>
-      <c r="Y103" s="9">
-        <v>1</v>
-      </c>
-      <c r="Z103" s="9">
-        <v>1</v>
-      </c>
-      <c r="AA103" s="9">
+        <f>COUNTIF(X100:X102,"Y")/3</f>
+        <v>1</v>
+      </c>
+      <c r="Y103" s="7">
+        <f t="shared" ref="Y103:AA103" si="43">COUNTIF(Y100:Y102,"Y")/3</f>
+        <v>1</v>
+      </c>
+      <c r="Z103" s="7">
+        <f t="shared" si="43"/>
+        <v>1</v>
+      </c>
+      <c r="AA103" s="7">
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
     </row>
@@ -10773,29 +11179,37 @@
       <c r="D105" s="2"/>
       <c r="E105" s="2"/>
       <c r="F105" s="7">
-        <v>1</v>
-      </c>
-      <c r="G105" s="9">
-        <v>1</v>
-      </c>
-      <c r="H105" s="9">
-        <v>1</v>
-      </c>
-      <c r="I105" s="9">
-        <v>0.67</v>
-      </c>
-      <c r="J105" s="9">
-        <v>0</v>
-      </c>
-      <c r="K105" s="9"/>
-      <c r="L105" s="9">
-        <v>0.33</v>
-      </c>
-      <c r="M105" s="9">
-        <v>0.33</v>
-      </c>
-      <c r="N105" s="9">
-        <v>0.67</v>
+        <f>COUNTIF(F102:F104,"Y")/3</f>
+        <v>1</v>
+      </c>
+      <c r="G105" s="7">
+        <f t="shared" ref="G105:N105" si="44">COUNTIF(G102:G104,"Y")/3</f>
+        <v>1</v>
+      </c>
+      <c r="H105" s="7">
+        <f t="shared" si="44"/>
+        <v>1</v>
+      </c>
+      <c r="I105" s="7">
+        <f t="shared" si="44"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="J105" s="7">
+        <f t="shared" si="44"/>
+        <v>0</v>
+      </c>
+      <c r="K105" s="7"/>
+      <c r="L105" s="7">
+        <f t="shared" si="44"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="M105" s="7">
+        <f t="shared" si="44"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="N105" s="7">
+        <f t="shared" si="44"/>
+        <v>0.66666666666666663</v>
       </c>
       <c r="W105">
         <v>1</v>
@@ -10893,16 +11307,20 @@
       <c r="V107" s="2"/>
       <c r="W107" s="2"/>
       <c r="X107" s="7">
-        <v>1</v>
-      </c>
-      <c r="Y107" s="9">
-        <v>1</v>
-      </c>
-      <c r="Z107" s="9">
-        <v>1</v>
-      </c>
-      <c r="AA107" s="9">
-        <v>0.33</v>
+        <f>COUNTIF(X104:X106,"Y")/3</f>
+        <v>1</v>
+      </c>
+      <c r="Y107" s="7">
+        <f t="shared" ref="Y107:AA107" si="45">COUNTIF(Y104:Y106,"Y")/3</f>
+        <v>1</v>
+      </c>
+      <c r="Z107" s="7">
+        <f t="shared" si="45"/>
+        <v>1</v>
+      </c>
+      <c r="AA107" s="7">
+        <f t="shared" si="45"/>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="108" spans="4:27" x14ac:dyDescent="0.3">
@@ -10957,29 +11375,37 @@
       <c r="D109" s="5"/>
       <c r="E109" s="5"/>
       <c r="F109" s="7">
-        <v>1</v>
-      </c>
-      <c r="G109" s="9">
-        <v>1</v>
-      </c>
-      <c r="H109" s="9">
-        <v>1</v>
-      </c>
-      <c r="I109" s="9">
-        <v>0.67</v>
-      </c>
-      <c r="J109" s="9">
-        <v>0.33</v>
-      </c>
-      <c r="K109" s="9"/>
-      <c r="L109" s="9">
-        <v>1</v>
-      </c>
-      <c r="M109" s="9">
-        <v>0.67</v>
-      </c>
-      <c r="N109" s="9">
-        <v>0.67</v>
+        <f>COUNTIF(F106:F108,"Y")/3</f>
+        <v>1</v>
+      </c>
+      <c r="G109" s="7">
+        <f t="shared" ref="G109:N109" si="46">COUNTIF(G106:G108,"Y")/3</f>
+        <v>1</v>
+      </c>
+      <c r="H109" s="7">
+        <f t="shared" si="46"/>
+        <v>1</v>
+      </c>
+      <c r="I109" s="7">
+        <f t="shared" si="46"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="J109" s="7">
+        <f t="shared" si="46"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="K109" s="7"/>
+      <c r="L109" s="7">
+        <f t="shared" si="46"/>
+        <v>1</v>
+      </c>
+      <c r="M109" s="7">
+        <f t="shared" si="46"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="N109" s="7">
+        <f t="shared" si="46"/>
+        <v>0.66666666666666663</v>
       </c>
       <c r="W109">
         <v>1</v>
@@ -11003,29 +11429,37 @@
       </c>
       <c r="E110" s="2"/>
       <c r="F110" s="6">
-        <v>1</v>
-      </c>
-      <c r="G110" s="8">
-        <v>1</v>
-      </c>
-      <c r="H110" s="8">
-        <v>1</v>
-      </c>
-      <c r="I110" s="8">
+        <f>AVERAGE(F94:F109)</f>
+        <v>1</v>
+      </c>
+      <c r="G110" s="6">
+        <f t="shared" ref="G110:N110" si="47">AVERAGE(G94:G109)</f>
+        <v>1</v>
+      </c>
+      <c r="H110" s="6">
+        <f t="shared" si="47"/>
+        <v>1</v>
+      </c>
+      <c r="I110" s="6">
+        <f t="shared" si="47"/>
         <v>0.5</v>
       </c>
-      <c r="J110" s="8">
-        <v>0.16700000000000001</v>
-      </c>
-      <c r="K110" s="8"/>
-      <c r="L110" s="8">
-        <v>0.41699999999999998</v>
-      </c>
-      <c r="M110" s="8">
+      <c r="J110" s="6">
+        <f t="shared" si="47"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="K110" s="6"/>
+      <c r="L110" s="6">
+        <f t="shared" si="47"/>
+        <v>0.41666666666666663</v>
+      </c>
+      <c r="M110" s="6">
+        <f t="shared" si="47"/>
         <v>0.75</v>
       </c>
-      <c r="N110" s="8">
-        <v>0.75</v>
+      <c r="N110" s="6">
+        <f t="shared" si="47"/>
+        <v>0.74999999999999989</v>
       </c>
       <c r="W110">
         <v>2</v>
@@ -11047,15 +11481,19 @@
       <c r="V111" s="2"/>
       <c r="W111" s="2"/>
       <c r="X111" s="7">
-        <v>1</v>
-      </c>
-      <c r="Y111" s="9">
-        <v>1</v>
-      </c>
-      <c r="Z111" s="9">
-        <v>1</v>
-      </c>
-      <c r="AA111" s="9">
+        <f>COUNTIF(X108:X110,"Y")/3</f>
+        <v>1</v>
+      </c>
+      <c r="Y111" s="7">
+        <f t="shared" ref="Y111:AA111" si="48">COUNTIF(Y108:Y110,"Y")/3</f>
+        <v>1</v>
+      </c>
+      <c r="Z111" s="7">
+        <f t="shared" si="48"/>
+        <v>1</v>
+      </c>
+      <c r="AA111" s="7">
+        <f t="shared" si="48"/>
         <v>0</v>
       </c>
     </row>
@@ -11220,15 +11658,19 @@
       <c r="V115" s="5"/>
       <c r="W115" s="5"/>
       <c r="X115" s="7">
-        <v>1</v>
-      </c>
-      <c r="Y115" s="9">
-        <v>0.67</v>
-      </c>
-      <c r="Z115" s="9">
-        <v>0.67</v>
-      </c>
-      <c r="AA115" s="9">
+        <f>COUNTIF(X112:X114,"Y")/3</f>
+        <v>1</v>
+      </c>
+      <c r="Y115" s="7">
+        <f t="shared" ref="Y115:AA115" si="49">COUNTIF(Y112:Y114,"Y")/3</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="Z115" s="7">
+        <f t="shared" si="49"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="AA115" s="7">
+        <f t="shared" si="49"/>
         <v>0</v>
       </c>
     </row>
@@ -11261,49 +11703,61 @@
       <c r="N116" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="V116" s="2" t="s">
+      <c r="V116" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="W116" s="2"/>
-      <c r="X116" s="6">
-        <v>1</v>
-      </c>
-      <c r="Y116" s="8">
-        <v>0.91700000000000004</v>
-      </c>
-      <c r="Z116" s="8">
-        <v>0.91700000000000004</v>
-      </c>
-      <c r="AA116" s="8">
-        <v>8.3000000000000004E-2</v>
+      <c r="W116" s="13"/>
+      <c r="X116" s="14">
+        <f>AVERAGE(X100:X115)</f>
+        <v>1</v>
+      </c>
+      <c r="Y116" s="14">
+        <f t="shared" ref="Y116:AA116" si="50">AVERAGE(Y100:Y115)</f>
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="Z116" s="14">
+        <f t="shared" si="50"/>
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="AA116" s="14">
+        <f t="shared" si="50"/>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="117" spans="2:27" x14ac:dyDescent="0.3">
       <c r="D117" s="2"/>
       <c r="E117" s="2"/>
       <c r="F117" s="7">
-        <v>1</v>
-      </c>
-      <c r="G117" s="9">
-        <v>1</v>
-      </c>
-      <c r="H117" s="9">
-        <v>1</v>
-      </c>
-      <c r="I117" s="9">
-        <v>0</v>
-      </c>
-      <c r="J117" s="9">
-        <v>0</v>
-      </c>
-      <c r="K117" s="9"/>
-      <c r="L117" s="9">
-        <v>0</v>
-      </c>
-      <c r="M117" s="9">
-        <v>0</v>
-      </c>
-      <c r="N117" s="9">
+        <f>COUNTIF(F114:F116,"Y")/3</f>
+        <v>1</v>
+      </c>
+      <c r="G117" s="7">
+        <f t="shared" ref="G117:N117" si="51">COUNTIF(G114:G116,"Y")/3</f>
+        <v>1</v>
+      </c>
+      <c r="H117" s="7">
+        <f t="shared" si="51"/>
+        <v>1</v>
+      </c>
+      <c r="I117" s="7">
+        <f t="shared" si="51"/>
+        <v>0</v>
+      </c>
+      <c r="J117" s="7">
+        <f t="shared" si="51"/>
+        <v>0</v>
+      </c>
+      <c r="K117" s="7"/>
+      <c r="L117" s="7">
+        <f t="shared" si="51"/>
+        <v>0</v>
+      </c>
+      <c r="M117" s="7">
+        <f t="shared" si="51"/>
+        <v>0</v>
+      </c>
+      <c r="N117" s="7">
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
     </row>
@@ -11404,29 +11858,37 @@
       <c r="D121" s="2"/>
       <c r="E121" s="2"/>
       <c r="F121" s="7">
-        <v>1</v>
-      </c>
-      <c r="G121" s="9">
-        <v>1</v>
-      </c>
-      <c r="H121" s="9">
-        <v>1</v>
-      </c>
-      <c r="I121" s="9">
-        <v>0.33</v>
-      </c>
-      <c r="J121" s="9">
-        <v>0</v>
-      </c>
-      <c r="K121" s="9"/>
-      <c r="L121" s="9">
-        <v>0.67</v>
-      </c>
-      <c r="M121" s="9">
-        <v>0.33</v>
-      </c>
-      <c r="N121" s="9">
-        <v>0.67</v>
+        <f>COUNTIF(F118:F120,"Y")/3</f>
+        <v>1</v>
+      </c>
+      <c r="G121" s="7">
+        <f t="shared" ref="G121:N121" si="52">COUNTIF(G118:G120,"Y")/3</f>
+        <v>1</v>
+      </c>
+      <c r="H121" s="7">
+        <f t="shared" si="52"/>
+        <v>1</v>
+      </c>
+      <c r="I121" s="7">
+        <f t="shared" si="52"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="J121" s="7">
+        <f t="shared" si="52"/>
+        <v>0</v>
+      </c>
+      <c r="K121" s="7"/>
+      <c r="L121" s="7">
+        <f t="shared" si="52"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="M121" s="7">
+        <f t="shared" si="52"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="N121" s="7">
+        <f t="shared" si="52"/>
+        <v>0.66666666666666663</v>
       </c>
       <c r="V121" t="s">
         <v>0</v>
@@ -11586,29 +12048,37 @@
       <c r="D125" s="2"/>
       <c r="E125" s="2"/>
       <c r="F125" s="7">
-        <v>1</v>
-      </c>
-      <c r="G125" s="9">
-        <v>0.67</v>
-      </c>
-      <c r="H125" s="9">
-        <v>1</v>
-      </c>
-      <c r="I125" s="9">
-        <v>0.33</v>
-      </c>
-      <c r="J125" s="9">
-        <v>0.67</v>
-      </c>
-      <c r="K125" s="9"/>
-      <c r="L125" s="9">
-        <v>0</v>
-      </c>
-      <c r="M125" s="9">
-        <v>0.33</v>
-      </c>
-      <c r="N125" s="9">
-        <v>0.67</v>
+        <f>COUNTIF(F122:F124,"Y")/3</f>
+        <v>1</v>
+      </c>
+      <c r="G125" s="7">
+        <f t="shared" ref="G125:N125" si="53">COUNTIF(G122:G124,"Y")/3</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="H125" s="7">
+        <f t="shared" si="53"/>
+        <v>1</v>
+      </c>
+      <c r="I125" s="7">
+        <f t="shared" si="53"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="J125" s="7">
+        <f t="shared" si="53"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="K125" s="7"/>
+      <c r="L125" s="7">
+        <f t="shared" si="53"/>
+        <v>0</v>
+      </c>
+      <c r="M125" s="7">
+        <f t="shared" si="53"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="N125" s="7">
+        <f t="shared" si="53"/>
+        <v>0.66666666666666663</v>
       </c>
       <c r="W125">
         <v>2</v>
@@ -11661,15 +12131,19 @@
       <c r="V126" s="2"/>
       <c r="W126" s="2"/>
       <c r="X126" s="7">
-        <v>1</v>
-      </c>
-      <c r="Y126" s="9">
-        <v>0.33</v>
-      </c>
-      <c r="Z126" s="9">
-        <v>0</v>
-      </c>
-      <c r="AA126" s="9">
+        <f>COUNTIF(X123:X125,"Y")/3</f>
+        <v>1</v>
+      </c>
+      <c r="Y126" s="7">
+        <f t="shared" ref="Y126:AA126" si="54">COUNTIF(Y123:Y125,"Y")/3</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="Z126" s="7">
+        <f t="shared" si="54"/>
+        <v>0</v>
+      </c>
+      <c r="AA126" s="7">
+        <f t="shared" si="54"/>
         <v>0</v>
       </c>
     </row>
@@ -11766,33 +12240,41 @@
         <v>17</v>
       </c>
     </row>
-    <row r="129" spans="4:27" x14ac:dyDescent="0.3">
+    <row r="129" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D129" s="5"/>
       <c r="E129" s="5"/>
       <c r="F129" s="7">
-        <v>1</v>
-      </c>
-      <c r="G129" s="9">
-        <v>0.67</v>
-      </c>
-      <c r="H129" s="9">
-        <v>1</v>
-      </c>
-      <c r="I129" s="9">
-        <v>0.67</v>
-      </c>
-      <c r="J129" s="9">
-        <v>0</v>
-      </c>
-      <c r="K129" s="9"/>
-      <c r="L129" s="9">
-        <v>0.33</v>
-      </c>
-      <c r="M129" s="9">
-        <v>0</v>
-      </c>
-      <c r="N129" s="9">
-        <v>0.67</v>
+        <f>COUNTIF(F126:F128,"Y")/3</f>
+        <v>1</v>
+      </c>
+      <c r="G129" s="7">
+        <f t="shared" ref="G129:N129" si="55">COUNTIF(G126:G128,"Y")/3</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="H129" s="7">
+        <f t="shared" si="55"/>
+        <v>1</v>
+      </c>
+      <c r="I129" s="7">
+        <f t="shared" si="55"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="J129" s="7">
+        <f t="shared" si="55"/>
+        <v>0</v>
+      </c>
+      <c r="K129" s="7"/>
+      <c r="L129" s="7">
+        <f t="shared" si="55"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="M129" s="7">
+        <f t="shared" si="55"/>
+        <v>0</v>
+      </c>
+      <c r="N129" s="7">
+        <f t="shared" si="55"/>
+        <v>0.66666666666666663</v>
       </c>
       <c r="W129">
         <v>2</v>
@@ -11810,52 +12292,64 @@
         <v>17</v>
       </c>
     </row>
-    <row r="130" spans="4:27" x14ac:dyDescent="0.3">
+    <row r="130" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D130" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E130" s="2"/>
       <c r="F130" s="6">
-        <v>1</v>
-      </c>
-      <c r="G130" s="8">
-        <v>0.83299999999999996</v>
-      </c>
-      <c r="H130" s="8">
-        <v>1</v>
-      </c>
-      <c r="I130" s="8">
-        <v>0.33300000000000002</v>
-      </c>
-      <c r="J130" s="8">
-        <v>0.16700000000000001</v>
-      </c>
-      <c r="K130" s="8"/>
-      <c r="L130" s="8">
+        <f>AVERAGE(F114:F129)</f>
+        <v>1</v>
+      </c>
+      <c r="G130" s="6">
+        <f t="shared" ref="G130:N130" si="56">AVERAGE(G114:G129)</f>
+        <v>0.83333333333333326</v>
+      </c>
+      <c r="H130" s="6">
+        <f t="shared" si="56"/>
+        <v>1</v>
+      </c>
+      <c r="I130" s="6">
+        <f t="shared" si="56"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="J130" s="6">
+        <f t="shared" si="56"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="K130" s="6"/>
+      <c r="L130" s="6">
+        <f t="shared" si="56"/>
         <v>0.25</v>
       </c>
-      <c r="M130" s="8">
-        <v>0.16700000000000001</v>
-      </c>
-      <c r="N130" s="8">
+      <c r="M130" s="6">
+        <f t="shared" si="56"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="N130" s="6">
+        <f t="shared" si="56"/>
         <v>0.5</v>
       </c>
       <c r="V130" s="2"/>
       <c r="W130" s="2"/>
       <c r="X130" s="7">
-        <v>1</v>
-      </c>
-      <c r="Y130" s="9">
-        <v>1</v>
-      </c>
-      <c r="Z130" s="9">
-        <v>0.67</v>
-      </c>
-      <c r="AA130" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="131" spans="4:27" x14ac:dyDescent="0.3">
+        <f>COUNTIF(X127:X129,"Y")/3</f>
+        <v>1</v>
+      </c>
+      <c r="Y130" s="7">
+        <f t="shared" ref="Y130:AA130" si="57">COUNTIF(Y127:Y129,"Y")/3</f>
+        <v>1</v>
+      </c>
+      <c r="Z130" s="7">
+        <f t="shared" si="57"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="AA130" s="7">
+        <f t="shared" si="57"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="4:32" x14ac:dyDescent="0.3">
       <c r="V131">
         <v>0.7</v>
       </c>
@@ -11875,7 +12369,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="132" spans="4:27" x14ac:dyDescent="0.3">
+    <row r="132" spans="4:32" x14ac:dyDescent="0.3">
       <c r="W132">
         <v>1</v>
       </c>
@@ -11892,7 +12386,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="133" spans="4:27" x14ac:dyDescent="0.3">
+    <row r="133" spans="4:32" x14ac:dyDescent="0.3">
       <c r="W133">
         <v>2</v>
       </c>
@@ -11909,23 +12403,27 @@
         <v>17</v>
       </c>
     </row>
-    <row r="134" spans="4:27" x14ac:dyDescent="0.3">
+    <row r="134" spans="4:32" x14ac:dyDescent="0.3">
       <c r="V134" s="2"/>
       <c r="W134" s="2"/>
       <c r="X134" s="7">
-        <v>1</v>
-      </c>
-      <c r="Y134" s="9">
-        <v>0.33</v>
-      </c>
-      <c r="Z134" s="9">
-        <v>0.33</v>
-      </c>
-      <c r="AA134" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="135" spans="4:27" x14ac:dyDescent="0.3">
+        <f>COUNTIF(X131:X133,"Y")/3</f>
+        <v>1</v>
+      </c>
+      <c r="Y134" s="7">
+        <f t="shared" ref="Y134:AA134" si="58">COUNTIF(Y131:Y133,"Y")/3</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="Z134" s="7">
+        <f t="shared" si="58"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="AA134" s="7">
+        <f t="shared" si="58"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D135" t="s">
         <v>28</v>
       </c>
@@ -11972,7 +12470,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="136" spans="4:27" x14ac:dyDescent="0.3">
+    <row r="136" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D136" t="s">
         <v>29</v>
       </c>
@@ -12016,7 +12514,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="137" spans="4:27" x14ac:dyDescent="0.3">
+    <row r="137" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D137" t="s">
         <v>30</v>
       </c>
@@ -12060,7 +12558,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="138" spans="4:27" x14ac:dyDescent="0.3">
+    <row r="138" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D138" t="s">
         <v>31</v>
       </c>
@@ -12091,19 +12589,23 @@
       <c r="V138" s="5"/>
       <c r="W138" s="5"/>
       <c r="X138" s="7">
-        <v>1</v>
-      </c>
-      <c r="Y138" s="9">
-        <v>0.67</v>
-      </c>
-      <c r="Z138" s="9">
-        <v>0.33</v>
-      </c>
-      <c r="AA138" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="139" spans="4:27" x14ac:dyDescent="0.3">
+        <f>COUNTIF(X135:X137,"Y")/3</f>
+        <v>1</v>
+      </c>
+      <c r="Y138" s="7">
+        <f t="shared" ref="Y138:AA138" si="59">COUNTIF(Y135:Y137,"Y")/3</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="Z138" s="7">
+        <f t="shared" si="59"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="AA138" s="7">
+        <f t="shared" si="59"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D139" t="s">
         <v>2</v>
       </c>
@@ -12131,24 +12633,32 @@
       <c r="N139">
         <v>0</v>
       </c>
-      <c r="V139" s="2" t="s">
+      <c r="V139" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="W139" s="2"/>
-      <c r="X139" s="6">
-        <v>1</v>
-      </c>
-      <c r="Y139" s="8">
-        <v>0.58299999999999996</v>
-      </c>
-      <c r="Z139" s="8">
-        <v>0.33300000000000002</v>
-      </c>
-      <c r="AA139" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="140" spans="4:27" x14ac:dyDescent="0.3">
+      <c r="W139" s="13"/>
+      <c r="X139" s="14">
+        <f>AVERAGE(X123:X138)</f>
+        <v>1</v>
+      </c>
+      <c r="Y139" s="14">
+        <f t="shared" ref="Y139:AA139" si="60">AVERAGE(Y123:Y138)</f>
+        <v>0.58333333333333326</v>
+      </c>
+      <c r="Z139" s="14">
+        <f t="shared" si="60"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="AA139" s="14">
+        <f t="shared" si="60"/>
+        <v>0</v>
+      </c>
+      <c r="AC139" s="16"/>
+      <c r="AD139" s="17"/>
+      <c r="AE139" s="16"/>
+      <c r="AF139" s="16"/>
+    </row>
+    <row r="140" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D140" t="s">
         <v>32</v>
       </c>
@@ -12176,8 +12686,9 @@
       <c r="N140">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="141" spans="4:27" x14ac:dyDescent="0.3">
+      <c r="X140" s="15"/>
+    </row>
+    <row r="141" spans="4:32" x14ac:dyDescent="0.3">
       <c r="D141" t="s">
         <v>4</v>
       </c>
@@ -12206,7 +12717,7 @@
         <v>0.66666666699999999</v>
       </c>
     </row>
-    <row r="142" spans="4:27" x14ac:dyDescent="0.3">
+    <row r="142" spans="4:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D142" t="s">
         <v>33</v>
       </c>
@@ -12235,17 +12746,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="4:27" x14ac:dyDescent="0.3">
-      <c r="X144" t="s">
+    <row r="143" spans="4:32" x14ac:dyDescent="0.3">
+      <c r="W143" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="X143" s="28"/>
+      <c r="Y143" s="28"/>
+      <c r="Z143" s="28"/>
+      <c r="AA143" s="29"/>
+    </row>
+    <row r="144" spans="4:32" x14ac:dyDescent="0.3">
+      <c r="W144" s="20"/>
+      <c r="X144" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="Y144" t="s">
+      <c r="Y144" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="Z144" t="s">
+      <c r="Z144" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="AA144" t="s">
+      <c r="AA144" s="30" t="s">
         <v>21</v>
       </c>
     </row>
@@ -12274,19 +12795,29 @@
       <c r="N145" t="s">
         <v>9</v>
       </c>
-      <c r="W145" t="s">
+      <c r="W145" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="X145" s="12">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="Y145" s="12">
-        <v>0.89</v>
-      </c>
-      <c r="Z145" s="12">
-        <v>0.39</v>
-      </c>
-      <c r="AA145" s="12">
+      <c r="X145" s="22">
+        <f>SUM(COUNTIF(X11:X13,"Y"),COUNTIF(X33:X35,"Y"),COUNTIF(X55:X57,"Y"),COUNTIF(X77:X79,"Y"),COUNTIF(X100:X102,"Y"),COUNTIF(X123:X125,"Y"))
+/
+SUM(COUNTIF(X11:X13,"Y"),COUNTIF(X11:X13,"N"),COUNTIF(X33:X35,"Y"),COUNTIF(X33:X35,"N"),COUNTIF(X55:X57,"Y"),COUNTIF(X55:X57,"N"),COUNTIF(X77:X79,"Y"),COUNTIF(X77:X79,"N"),COUNTIF(X100:X102,"Y"),COUNTIF(X100:X102,"N"),COUNTIF(X123:X125,"Y"),COUNTIF(X123:X125,"N"))</f>
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="Y145" s="22">
+        <f>SUM(COUNTIF(Y11:Y13,"Y"),COUNTIF(Y33:Y35,"Y"),COUNTIF(Y55:Y57,"Y"),COUNTIF(Y77:Y79,"Y"),COUNTIF(Y100:Y102,"Y"),COUNTIF(Y123:Y125,"Y"))
+/
+SUM(COUNTIF(Y11:Y13,"Y"),COUNTIF(Y11:Y13,"N"),COUNTIF(Y33:Y35,"Y"),COUNTIF(Y33:Y35,"N"),COUNTIF(Y55:Y57,"Y"),COUNTIF(Y55:Y57,"N"),COUNTIF(Y77:Y79,"Y"),COUNTIF(Y77:Y79,"N"),COUNTIF(Y100:Y102,"Y"),COUNTIF(Y100:Y102,"N"),COUNTIF(Y123:Y125,"Y"),COUNTIF(Y123:Y125,"N"))</f>
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="Z145" s="22">
+        <f t="shared" ref="Z145:AA145" si="61">SUM(COUNTIF(Z11:Z13,"Y"),COUNTIF(Z33:Z35,"Y"),COUNTIF(Z55:Z57,"Y"),COUNTIF(Z77:Z79,"Y"),COUNTIF(Z100:Z102,"Y"),COUNTIF(Z123:Z125,"Y"))
+/
+SUM(COUNTIF(Z11:Z13,"Y"),COUNTIF(Z11:Z13,"N"),COUNTIF(Z33:Z35,"Y"),COUNTIF(Z33:Z35,"N"),COUNTIF(Z55:Z57,"Y"),COUNTIF(Z55:Z57,"N"),COUNTIF(Z77:Z79,"Y"),COUNTIF(Z77:Z79,"N"),COUNTIF(Z100:Z102,"Y"),COUNTIF(Z100:Z102,"N"),COUNTIF(Z123:Z125,"Y"),COUNTIF(Z123:Z125,"N"))</f>
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="AA145" s="23">
+        <f t="shared" si="61"/>
         <v>0</v>
       </c>
     </row>
@@ -12321,20 +12852,32 @@
       <c r="N146">
         <v>0</v>
       </c>
-      <c r="W146" t="s">
+      <c r="W146" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="X146" s="12">
-        <v>0.67</v>
-      </c>
-      <c r="Y146" s="12">
-        <v>0.94</v>
-      </c>
-      <c r="Z146" s="12">
-        <v>0.61</v>
-      </c>
-      <c r="AA146" s="12">
-        <v>0.06</v>
+      <c r="X146" s="22">
+        <f>SUM(COUNTIF(X15:X17,"Y"),COUNTIF(X37:X39,"Y"),COUNTIF(X59:X61,"Y"),COUNTIF(X81:X83,"Y"),COUNTIF(X104:X106,"Y"),COUNTIF(X127:X129,"Y"))
+/
+SUM(COUNTIF(X15:X17,"Y"),COUNTIF(X15:X17,"N"),COUNTIF(X37:X39,"Y"),COUNTIF(X37:X39,"N"),COUNTIF(X59:X61,"Y"),COUNTIF(X59:X61,"N"),COUNTIF(X81:X83,"Y"),COUNTIF(X81:X83,"N"),COUNTIF(X104:X106,"Y"),COUNTIF(X104:X106,"N"),COUNTIF(X127:X129,"Y"),COUNTIF(X127:X129,"N"))</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="Y146" s="22">
+        <f>SUM(COUNTIF(Y15:Y17,"Y"),COUNTIF(Y37:Y39,"Y"),COUNTIF(Y59:Y61,"Y"),COUNTIF(Y81:Y83,"Y"),COUNTIF(Y104:Y106,"Y"),COUNTIF(Y127:Y129,"Y"))
+/
+SUM(COUNTIF(Y15:Y17,"Y"),COUNTIF(Y15:Y17,"N"),COUNTIF(Y37:Y39,"Y"),COUNTIF(Y37:Y39,"N"),COUNTIF(Y59:Y61,"Y"),COUNTIF(Y59:Y61,"N"),COUNTIF(Y81:Y83,"Y"),COUNTIF(Y81:Y83,"N"),COUNTIF(Y104:Y106,"Y"),COUNTIF(Y104:Y106,"N"),COUNTIF(Y127:Y129,"Y"),COUNTIF(Y127:Y129,"N"))</f>
+        <v>0.94444444444444442</v>
+      </c>
+      <c r="Z146" s="22">
+        <f>SUM(COUNTIF(Z15:Z17,"Y"),COUNTIF(Z37:Z39,"Y"),COUNTIF(Z59:Z61,"Y"),COUNTIF(Z81:Z83,"Y"),COUNTIF(Z104:Z106,"Y"),COUNTIF(Z127:Z129,"Y"))
+/
+SUM(COUNTIF(Z15:Z17,"Y"),COUNTIF(Z15:Z17,"N"),COUNTIF(Z37:Z39,"Y"),COUNTIF(Z37:Z39,"N"),COUNTIF(Z59:Z61,"Y"),COUNTIF(Z59:Z61,"N"),COUNTIF(Z81:Z83,"Y"),COUNTIF(Z81:Z83,"N"),COUNTIF(Z104:Z106,"Y"),COUNTIF(Z104:Z106,"N"),COUNTIF(Z127:Z129,"Y"),COUNTIF(Z127:Z129,"N"))</f>
+        <v>0.61111111111111116</v>
+      </c>
+      <c r="AA146" s="23">
+        <f>SUM(COUNTIF(AA15:AA17,"Y"),COUNTIF(AA37:AA39,"Y"),COUNTIF(AA59:AA61,"Y"),COUNTIF(AA81:AA83,"Y"),COUNTIF(AA104:AA106,"Y"),COUNTIF(AA127:AA129,"Y"))
+/
+SUM(COUNTIF(AA15:AA17,"Y"),COUNTIF(AA15:AA17,"N"),COUNTIF(AA37:AA39,"Y"),COUNTIF(AA37:AA39,"N"),COUNTIF(AA59:AA61,"Y"),COUNTIF(AA59:AA61,"N"),COUNTIF(AA81:AA83,"Y"),COUNTIF(AA81:AA83,"N"),COUNTIF(AA104:AA106,"Y"),COUNTIF(AA104:AA106,"N"),COUNTIF(AA127:AA129,"Y"),COUNTIF(AA127:AA129,"N"))</f>
+        <v>5.5555555555555552E-2</v>
       </c>
     </row>
     <row r="147" spans="4:27" x14ac:dyDescent="0.3">
@@ -12365,23 +12908,35 @@
       <c r="N147">
         <v>0.5</v>
       </c>
-      <c r="W147" t="s">
+      <c r="W147" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="X147" s="12">
-        <v>0.72</v>
-      </c>
-      <c r="Y147" s="12">
-        <v>0.89</v>
-      </c>
-      <c r="Z147" s="12">
-        <v>0.61</v>
-      </c>
-      <c r="AA147" s="12">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="148" spans="4:27" x14ac:dyDescent="0.3">
+      <c r="X147" s="22">
+        <f>SUM(COUNTIF(X19:X21,"Y"),COUNTIF(X41:X43,"Y"),COUNTIF(X63:X65,"Y"),COUNTIF(X85:X87,"Y"),COUNTIF(X108:X110,"Y"),COUNTIF(X131:X133,"Y"))
+/
+SUM(COUNTIF(X19:X21,"Y"),COUNTIF(X19:X21,"N"),COUNTIF(X41:X43,"Y"),COUNTIF(X41:X43,"N"),COUNTIF(X63:X65,"Y"),COUNTIF(X63:X65,"N"),COUNTIF(X85:X87,"Y"),COUNTIF(X85:X87,"N"),COUNTIF(X108:X110,"Y"),COUNTIF(X108:X110,"N"),COUNTIF(X131:X133,"Y"),COUNTIF(X131:X133,"N"))</f>
+        <v>0.72222222222222221</v>
+      </c>
+      <c r="Y147" s="22">
+        <f>SUM(COUNTIF(Y19:Y21,"Y"),COUNTIF(Y41:Y43,"Y"),COUNTIF(Y63:Y65,"Y"),COUNTIF(Y85:Y87,"Y"),COUNTIF(Y108:Y110,"Y"),COUNTIF(Y131:Y133,"Y"))
+/
+SUM(COUNTIF(Y19:Y21,"Y"),COUNTIF(Y19:Y21,"N"),COUNTIF(Y41:Y43,"Y"),COUNTIF(Y41:Y43,"N"),COUNTIF(Y63:Y65,"Y"),COUNTIF(Y63:Y65,"N"),COUNTIF(Y85:Y87,"Y"),COUNTIF(Y85:Y87,"N"),COUNTIF(Y108:Y110,"Y"),COUNTIF(Y108:Y110,"N"),COUNTIF(Y131:Y133,"Y"),COUNTIF(Y131:Y133,"N"))</f>
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="Z147" s="22">
+        <f>SUM(COUNTIF(Z19:Z21,"Y"),COUNTIF(Z41:Z43,"Y"),COUNTIF(Z63:Z65,"Y"),COUNTIF(Z85:Z87,"Y"),COUNTIF(Z108:Z110,"Y"),COUNTIF(Z131:Z133,"Y"))
+/
+SUM(COUNTIF(Z19:Z21,"Y"),COUNTIF(Z19:Z21,"N"),COUNTIF(Z41:Z43,"Y"),COUNTIF(Z41:Z43,"N"),COUNTIF(Z63:Z65,"Y"),COUNTIF(Z63:Z65,"N"),COUNTIF(Z85:Z87,"Y"),COUNTIF(Z85:Z87,"N"),COUNTIF(Z108:Z110,"Y"),COUNTIF(Z108:Z110,"N"),COUNTIF(Z131:Z133,"Y"),COUNTIF(Z131:Z133,"N"))</f>
+        <v>0.61111111111111116</v>
+      </c>
+      <c r="AA147" s="23">
+        <f>SUM(COUNTIF(AA19:AA21,"Y"),COUNTIF(AA41:AA43,"Y"),COUNTIF(AA63:AA65,"Y"),COUNTIF(AA85:AA87,"Y"),COUNTIF(AA108:AA110,"Y"),COUNTIF(AA131:AA133,"Y"))
+/
+SUM(COUNTIF(AA19:AA21,"Y"),COUNTIF(AA19:AA21,"N"),COUNTIF(AA41:AA43,"Y"),COUNTIF(AA41:AA43,"N"),COUNTIF(AA63:AA65,"Y"),COUNTIF(AA63:AA65,"N"),COUNTIF(AA85:AA87,"Y"),COUNTIF(AA85:AA87,"N"),COUNTIF(AA108:AA110,"Y"),COUNTIF(AA108:AA110,"N"),COUNTIF(AA131:AA133,"Y"),COUNTIF(AA131:AA133,"N"))</f>
+        <v>5.5555555555555552E-2</v>
+      </c>
+    </row>
+    <row r="148" spans="4:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E148" t="s">
         <v>40</v>
       </c>
@@ -12409,20 +12964,32 @@
       <c r="N148">
         <v>0.16666666699999999</v>
       </c>
-      <c r="W148" t="s">
+      <c r="W148" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="X148" s="12">
-        <v>0.78</v>
-      </c>
-      <c r="Y148" s="12">
-        <v>0.89</v>
-      </c>
-      <c r="Z148" s="12">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="AA148" s="12">
-        <v>0.06</v>
+      <c r="X148" s="26">
+        <f>SUM(COUNTIF(X23:X25,"Y"),COUNTIF(X45:X47,"Y"),COUNTIF(X67:X69,"Y"),COUNTIF(X89:X91,"Y"),COUNTIF(X112:X114,"Y"),COUNTIF(X135:X137,"Y"))
+/
+SUM(COUNTIF(X23:X25,"Y"),COUNTIF(X23:X25,"N"),COUNTIF(X45:X47,"Y"),COUNTIF(X45:X47,"N"),COUNTIF(X67:X69,"Y"),COUNTIF(X67:X69,"N"),COUNTIF(X89:X91,"Y"),COUNTIF(X89:X91,"N"),COUNTIF(X112:X114,"Y"),COUNTIF(X112:X114,"N"),COUNTIF(X135:X137,"Y"),COUNTIF(X135:X137,"N"))</f>
+        <v>0.77777777777777779</v>
+      </c>
+      <c r="Y148" s="26">
+        <f>SUM(COUNTIF(Y23:Y25,"Y"),COUNTIF(Y45:Y47,"Y"),COUNTIF(Y67:Y69,"Y"),COUNTIF(Y89:Y91,"Y"),COUNTIF(Y112:Y114,"Y"),COUNTIF(Y135:Y137,"Y"))
+/
+SUM(COUNTIF(Y23:Y25,"Y"),COUNTIF(Y23:Y25,"N"),COUNTIF(Y45:Y47,"Y"),COUNTIF(Y45:Y47,"N"),COUNTIF(Y67:Y69,"Y"),COUNTIF(Y67:Y69,"N"),COUNTIF(Y89:Y91,"Y"),COUNTIF(Y89:Y91,"N"),COUNTIF(Y112:Y114,"Y"),COUNTIF(Y112:Y114,"N"),COUNTIF(Y135:Y137,"Y"),COUNTIF(Y135:Y137,"N"))</f>
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="Z148" s="26">
+        <f>SUM(COUNTIF(Z23:Z25,"Y"),COUNTIF(Z45:Z47,"Y"),COUNTIF(Z67:Z69,"Y"),COUNTIF(Z89:Z91,"Y"),COUNTIF(Z112:Z114,"Y"),COUNTIF(Z135:Z137,"Y"))
+/
+SUM(COUNTIF(Z23:Z25,"Y"),COUNTIF(Z23:Z25,"N"),COUNTIF(Z45:Z47,"Y"),COUNTIF(Z45:Z47,"N"),COUNTIF(Z67:Z69,"Y"),COUNTIF(Z67:Z69,"N"),COUNTIF(Z89:Z91,"Y"),COUNTIF(Z89:Z91,"N"),COUNTIF(Z112:Z114,"Y"),COUNTIF(Z112:Z114,"N"),COUNTIF(Z135:Z137,"Y"),COUNTIF(Z135:Z137,"N"))</f>
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="AA148" s="27">
+        <f>SUM(COUNTIF(AA23:AA25,"Y"),COUNTIF(AA45:AA47,"Y"),COUNTIF(AA67:AA69,"Y"),COUNTIF(AA89:AA91,"Y"),COUNTIF(AA112:AA114,"Y"),COUNTIF(AA135:AA137,"Y"))
+/
+SUM(COUNTIF(AA23:AA25,"Y"),COUNTIF(AA23:AA25,"N"),COUNTIF(AA45:AA47,"Y"),COUNTIF(AA45:AA47,"N"),COUNTIF(AA67:AA69,"Y"),COUNTIF(AA67:AA69,"N"),COUNTIF(AA89:AA91,"Y"),COUNTIF(AA89:AA91,"N"),COUNTIF(AA112:AA114,"Y"),COUNTIF(AA112:AA114,"N"),COUNTIF(AA135:AA137,"Y"),COUNTIF(AA135:AA137,"N"))</f>
+        <v>5.5555555555555552E-2</v>
       </c>
     </row>
     <row r="149" spans="4:27" x14ac:dyDescent="0.3">
@@ -12455,325 +13022,418 @@
       </c>
     </row>
     <row r="151" spans="4:27" x14ac:dyDescent="0.3">
-      <c r="X151" s="12">
+      <c r="X151" s="18">
         <v>0.5</v>
       </c>
-      <c r="Y151" s="12">
+      <c r="Y151" s="18">
         <v>0.27</v>
       </c>
-      <c r="Z151" s="12">
+      <c r="Z151" s="18">
         <v>0.49</v>
       </c>
-      <c r="AA151" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="152" spans="4:27" x14ac:dyDescent="0.3">
-      <c r="X152" s="12">
+      <c r="AA151" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="4:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="X152" s="18">
         <v>0.42</v>
       </c>
-      <c r="Y152" s="12">
+      <c r="Y152" s="18">
         <v>0.14000000000000001</v>
       </c>
-      <c r="Z152" s="12">
+      <c r="Z152" s="18">
         <v>0.39</v>
       </c>
-      <c r="AA152" s="12">
+      <c r="AA152" s="18">
         <v>0.14000000000000001</v>
       </c>
     </row>
     <row r="153" spans="4:27" x14ac:dyDescent="0.3">
-      <c r="X153" s="12">
+      <c r="D153" s="19"/>
+      <c r="E153" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="F153" s="28"/>
+      <c r="G153" s="28"/>
+      <c r="H153" s="28"/>
+      <c r="I153" s="28"/>
+      <c r="J153" s="28"/>
+      <c r="K153" s="28"/>
+      <c r="L153" s="28"/>
+      <c r="M153" s="28"/>
+      <c r="N153" s="29"/>
+      <c r="X153" s="18">
         <v>0.44</v>
       </c>
-      <c r="Y153" s="12">
+      <c r="Y153" s="18">
         <v>0.27</v>
       </c>
-      <c r="Z153" s="12">
+      <c r="Z153" s="18">
         <v>0.44</v>
       </c>
-      <c r="AA153" s="12">
+      <c r="AA153" s="18">
         <v>0.14000000000000001</v>
       </c>
     </row>
     <row r="154" spans="4:27" x14ac:dyDescent="0.3">
-      <c r="E154" t="s">
-        <v>43</v>
-      </c>
-      <c r="F154" t="s">
+      <c r="D154" s="31"/>
+      <c r="E154" s="32"/>
+      <c r="F154" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="G154" t="s">
+      <c r="G154" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="H154" t="s">
+      <c r="H154" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="I154" t="s">
+      <c r="I154" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="J154" t="s">
+      <c r="J154" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="L154" t="s">
+      <c r="K154" s="32"/>
+      <c r="L154" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="M154" t="s">
+      <c r="M154" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="N154" t="s">
+      <c r="N154" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="X154" s="12">
+      <c r="X154" s="18">
         <v>0.34</v>
       </c>
-      <c r="Y154" s="12">
+      <c r="Y154" s="18">
         <v>0.17</v>
       </c>
-      <c r="Z154" s="12">
+      <c r="Z154" s="18">
         <v>0.4</v>
       </c>
-      <c r="AA154" s="12">
+      <c r="AA154" s="18">
         <v>0.14000000000000001</v>
       </c>
     </row>
     <row r="155" spans="4:27" x14ac:dyDescent="0.3">
-      <c r="D155">
-        <v>0</v>
-      </c>
-      <c r="F155">
-        <v>1</v>
-      </c>
-      <c r="G155">
-        <v>0.77777777800000003</v>
-      </c>
-      <c r="H155">
-        <v>0.66666666699999999</v>
-      </c>
-      <c r="I155">
-        <v>0.16666666699999999</v>
-      </c>
-      <c r="J155">
-        <v>0.33333333300000001</v>
-      </c>
-      <c r="L155">
-        <v>0.66666666699999999</v>
-      </c>
-      <c r="M155">
-        <v>0.66666666699999999</v>
-      </c>
-      <c r="N155">
-        <v>0.44444444399999999</v>
+      <c r="D155" s="20">
+        <v>0</v>
+      </c>
+      <c r="E155" s="21"/>
+      <c r="F155" s="22">
+        <f>SUM(COUNTIF(F9:F11,"Y"),COUNTIF(F32:F34,"Y"),COUNTIF(F53:F55,"Y"),COUNTIF(F74:F76,"Y"),COUNTIF(F94:F96,"Y"),COUNTIF(F114:F116,"Y"))
+/
+SUM(COUNTIF(F9:F11,"Y"),COUNTIF(F9:F11,"N"),COUNTIF(F32:F34,"Y"),COUNTIF(F32:F34,"N"),COUNTIF(F53:F55,"Y"),COUNTIF(F53:F55,"N"),COUNTIF(F74:F76,"Y"),COUNTIF(F74:F76,"N"),COUNTIF(F94:F96,"Y"),COUNTIF(F94:F96,"N"),COUNTIF(F114:F116,"Y"),COUNTIF(F114:F116,"N"))</f>
+        <v>1</v>
+      </c>
+      <c r="G155" s="22">
+        <f>SUM(COUNTIF(G9:G11,"Y"),COUNTIF(G32:G34,"Y"),COUNTIF(G53:G55,"Y"),COUNTIF(G74:G76,"Y"),COUNTIF(G94:G96,"Y"),COUNTIF(G114:G116,"Y"))
+/
+SUM(COUNTIF(G9:G11,"Y"),COUNTIF(G9:G11,"N"),COUNTIF(G32:G34,"Y"),COUNTIF(G32:G34,"N"),COUNTIF(G53:G55,"Y"),COUNTIF(G53:G55,"N"),COUNTIF(G74:G76,"Y"),COUNTIF(G74:G76,"N"),COUNTIF(G94:G96,"Y"),COUNTIF(G94:G96,"N"),COUNTIF(G114:G116,"Y"),COUNTIF(G114:G116,"N"))</f>
+        <v>0.77777777777777779</v>
+      </c>
+      <c r="H155" s="22">
+        <f>SUM(COUNTIF(H9:H11,"Y"),COUNTIF(H32:H34,"Y"),COUNTIF(H53:H55,"Y"),COUNTIF(H74:H76,"Y"),COUNTIF(H94:H96,"Y"),COUNTIF(H114:H116,"Y"))
+/
+SUM(COUNTIF(H9:H11,"Y"),COUNTIF(H9:H11,"N"),COUNTIF(H32:H34,"Y"),COUNTIF(H32:H34,"N"),COUNTIF(H53:H55,"Y"),COUNTIF(H53:H55,"N"),COUNTIF(H74:H76,"Y"),COUNTIF(H74:H76,"N"),COUNTIF(H94:H96,"Y"),COUNTIF(H94:H96,"N"),COUNTIF(H114:H116,"Y"),COUNTIF(H114:H116,"N"))</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="I155" s="22">
+        <f>SUM(COUNTIF(I9:I11,"Y"),COUNTIF(I32:I34,"Y"),COUNTIF(I53:I55,"Y"),COUNTIF(I74:I76,"Y"),COUNTIF(I94:I96,"Y"),COUNTIF(I114:I116,"Y"))
+/
+SUM(COUNTIF(I9:I11,"Y"),COUNTIF(I9:I11,"N"),COUNTIF(I32:I34,"Y"),COUNTIF(I32:I34,"N"),COUNTIF(I53:I55,"Y"),COUNTIF(I53:I55,"N"),COUNTIF(I74:I76,"Y"),COUNTIF(I74:I76,"N"),COUNTIF(I94:I96,"Y"),COUNTIF(I94:I96,"N"),COUNTIF(I114:I116,"Y"),COUNTIF(I114:I116,"N"))</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="J155" s="22">
+        <f>SUM(COUNTIF(J9:J11,"Y"),COUNTIF(J32:J34,"Y"),COUNTIF(J53:J55,"Y"),COUNTIF(J74:J76,"Y"),COUNTIF(J94:J96,"Y"),COUNTIF(J114:J116,"Y"))
+/
+SUM(COUNTIF(J9:J11,"Y"),COUNTIF(J9:J11,"N"),COUNTIF(J32:J34,"Y"),COUNTIF(J32:J34,"N"),COUNTIF(J53:J55,"Y"),COUNTIF(J53:J55,"N"),COUNTIF(J74:J76,"Y"),COUNTIF(J74:J76,"N"),COUNTIF(J94:J96,"Y"),COUNTIF(J94:J96,"N"),COUNTIF(J114:J116,"Y"),COUNTIF(J114:J116,"N"))</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="K155" s="22"/>
+      <c r="L155" s="22">
+        <f>SUM(COUNTIF(L9:L11,"Y"),COUNTIF(L32:L34,"Y"),COUNTIF(L53:L55,"Y"),COUNTIF(L74:L76,"Y"),COUNTIF(L94:L96,"Y"),COUNTIF(L114:L116,"Y"))
+/
+SUM(COUNTIF(L9:L11,"Y"),COUNTIF(L9:L11,"N"),COUNTIF(L32:L34,"Y"),COUNTIF(L32:L34,"N"),COUNTIF(L53:L55,"Y"),COUNTIF(L53:L55,"N"),COUNTIF(L74:L76,"Y"),COUNTIF(L74:L76,"N"),COUNTIF(L94:L96,"Y"),COUNTIF(L94:L96,"N"),COUNTIF(L114:L116,"Y"),COUNTIF(L114:L116,"N"))</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="M155" s="22">
+        <f>SUM(COUNTIF(M9:M11,"Y"),COUNTIF(M32:M34,"Y"),COUNTIF(M53:M55,"Y"),COUNTIF(M74:M76,"Y"),COUNTIF(M94:M96,"Y"),COUNTIF(M114:M116,"Y"))
+/
+SUM(COUNTIF(M9:M11,"Y"),COUNTIF(M9:M11,"N"),COUNTIF(M32:M34,"Y"),COUNTIF(M32:M34,"N"),COUNTIF(M53:M55,"Y"),COUNTIF(M53:M55,"N"),COUNTIF(M74:M76,"Y"),COUNTIF(M74:M76,"N"),COUNTIF(M94:M96,"Y"),COUNTIF(M94:M96,"N"),COUNTIF(M114:M116,"Y"),COUNTIF(M114:M116,"N"))</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="N155" s="23">
+        <f>SUM(COUNTIF(N9:N11,"Y"),COUNTIF(N32:N34,"Y"),COUNTIF(N53:N55,"Y"),COUNTIF(N74:N76,"Y"),COUNTIF(N94:N96,"Y"),COUNTIF(N114:N116,"Y"))
+/
+SUM(COUNTIF(N9:N11,"Y"),COUNTIF(N9:N11,"N"),COUNTIF(N32:N34,"Y"),COUNTIF(N32:N34,"N"),COUNTIF(N53:N55,"Y"),COUNTIF(N53:N55,"N"),COUNTIF(N74:N76,"Y"),COUNTIF(N74:N76,"N"),COUNTIF(N94:N96,"Y"),COUNTIF(N94:N96,"N"),COUNTIF(N114:N116,"Y"),COUNTIF(N114:N116,"N"))</f>
+        <v>0.44444444444444442</v>
       </c>
     </row>
     <row r="156" spans="4:27" x14ac:dyDescent="0.3">
-      <c r="D156">
+      <c r="D156" s="20">
         <v>0.3</v>
       </c>
-      <c r="F156">
-        <v>1</v>
-      </c>
-      <c r="G156">
-        <v>0.83333333300000001</v>
-      </c>
-      <c r="H156">
-        <v>0.72222222199999997</v>
-      </c>
-      <c r="I156">
-        <v>0.27777777799999998</v>
-      </c>
-      <c r="J156">
-        <v>0.44444444399999999</v>
-      </c>
-      <c r="L156">
-        <v>0.55555555599999995</v>
-      </c>
-      <c r="M156">
+      <c r="E156" s="21"/>
+      <c r="F156" s="22">
+        <f>SUM(COUNTIF(F13:F15,"Y"),COUNTIF(F36:F38,"Y"),COUNTIF(F57:F59,"Y"),COUNTIF(F78:F80,"Y"),COUNTIF(F98:F100,"Y"),COUNTIF(F118:F120,"Y"))
+/
+SUM(COUNTIF(F13:F15,"Y"),COUNTIF(F13:F15,"N"),COUNTIF(F36:F38,"Y"),COUNTIF(F36:F38,"N"),COUNTIF(F57:F59,"Y"),COUNTIF(F57:F59,"N"),COUNTIF(F78:F80,"Y"),COUNTIF(F78:F80,"N"),COUNTIF(F98:F100,"Y"),COUNTIF(F98:F100,"N"),COUNTIF(F118:F120,"Y"),COUNTIF(F118:F120,"N"))</f>
+        <v>1</v>
+      </c>
+      <c r="G156" s="22">
+        <f t="shared" ref="G156:N156" si="62">SUM(COUNTIF(G13:G15,"Y"),COUNTIF(G36:G38,"Y"),COUNTIF(G57:G59,"Y"),COUNTIF(G78:G80,"Y"),COUNTIF(G98:G100,"Y"),COUNTIF(G118:G120,"Y"))
+/
+SUM(COUNTIF(G13:G15,"Y"),COUNTIF(G13:G15,"N"),COUNTIF(G36:G38,"Y"),COUNTIF(G36:G38,"N"),COUNTIF(G57:G59,"Y"),COUNTIF(G57:G59,"N"),COUNTIF(G78:G80,"Y"),COUNTIF(G78:G80,"N"),COUNTIF(G98:G100,"Y"),COUNTIF(G98:G100,"N"),COUNTIF(G118:G120,"Y"),COUNTIF(G118:G120,"N"))</f>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="H156" s="22">
+        <f t="shared" si="62"/>
+        <v>0.72222222222222221</v>
+      </c>
+      <c r="I156" s="22">
+        <f t="shared" si="62"/>
+        <v>0.27777777777777779</v>
+      </c>
+      <c r="J156" s="22">
+        <f t="shared" si="62"/>
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="K156" s="22"/>
+      <c r="L156" s="22">
+        <f t="shared" si="62"/>
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="M156" s="22">
+        <f t="shared" si="62"/>
         <v>0.5</v>
       </c>
-      <c r="N156">
+      <c r="N156" s="23">
+        <f t="shared" si="62"/>
         <v>0.5</v>
       </c>
     </row>
     <row r="157" spans="4:27" x14ac:dyDescent="0.3">
-      <c r="D157">
+      <c r="D157" s="20">
         <v>0.7</v>
       </c>
-      <c r="F157">
-        <v>1</v>
-      </c>
-      <c r="G157">
-        <v>0.77777777800000003</v>
-      </c>
-      <c r="H157">
-        <v>0.83333333300000001</v>
-      </c>
-      <c r="I157">
-        <v>0.44444444399999999</v>
-      </c>
-      <c r="J157">
-        <v>0.55555555599999995</v>
-      </c>
-      <c r="L157">
-        <v>0.33333333300000001</v>
-      </c>
-      <c r="M157">
-        <v>0.55555555599999995</v>
-      </c>
-      <c r="N157">
-        <v>0.33333333300000001</v>
-      </c>
-    </row>
-    <row r="158" spans="4:27" x14ac:dyDescent="0.3">
-      <c r="D158">
-        <v>1</v>
-      </c>
-      <c r="F158">
-        <v>1</v>
-      </c>
-      <c r="G158">
-        <v>0.88888888899999996</v>
-      </c>
-      <c r="H158">
-        <v>0.88888888899999996</v>
-      </c>
-      <c r="I158">
+      <c r="E157" s="21"/>
+      <c r="F157" s="22">
+        <f>SUM(COUNTIF(F17:F19,"Y"),COUNTIF(F40:F42,"Y"),COUNTIF(F61:F63,"Y"),COUNTIF(F82:F84,"Y"),COUNTIF(F102:F104,"Y"),COUNTIF(F122:F124,"Y"))
+/
+SUM(COUNTIF(F17:F19,"Y"),COUNTIF(F17:F19,"N"),COUNTIF(F40:F42,"Y"),COUNTIF(F40:F42,"N"),COUNTIF(F61:F63,"Y"),COUNTIF(F61:F63,"N"),COUNTIF(F82:F84,"Y"),COUNTIF(F82:F84,"N"),COUNTIF(F102:F104,"Y"),COUNTIF(F102:F104,"N"),COUNTIF(F122:F124,"Y"),COUNTIF(F122:F124,"N"))</f>
+        <v>1</v>
+      </c>
+      <c r="G157" s="22">
+        <f t="shared" ref="G157:N157" si="63">SUM(COUNTIF(G17:G19,"Y"),COUNTIF(G40:G42,"Y"),COUNTIF(G61:G63,"Y"),COUNTIF(G82:G84,"Y"),COUNTIF(G102:G104,"Y"),COUNTIF(G122:G124,"Y"))
+/
+SUM(COUNTIF(G17:G19,"Y"),COUNTIF(G17:G19,"N"),COUNTIF(G40:G42,"Y"),COUNTIF(G40:G42,"N"),COUNTIF(G61:G63,"Y"),COUNTIF(G61:G63,"N"),COUNTIF(G82:G84,"Y"),COUNTIF(G82:G84,"N"),COUNTIF(G102:G104,"Y"),COUNTIF(G102:G104,"N"),COUNTIF(G122:G124,"Y"),COUNTIF(G122:G124,"N"))</f>
+        <v>0.77777777777777779</v>
+      </c>
+      <c r="H157" s="22">
+        <f t="shared" si="63"/>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="I157" s="22">
+        <f t="shared" si="63"/>
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="J157" s="22">
+        <f t="shared" si="63"/>
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="K157" s="22"/>
+      <c r="L157" s="22">
+        <f t="shared" si="63"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="M157" s="22">
+        <f t="shared" si="63"/>
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="N157" s="23">
+        <f t="shared" si="63"/>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="158" spans="4:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D158" s="24">
+        <v>1</v>
+      </c>
+      <c r="E158" s="25"/>
+      <c r="F158" s="26">
+        <f>SUM(COUNTIF(F21:F23,"Y"),COUNTIF(F44:F46,"Y"),COUNTIF(F65:F67,"Y"),COUNTIF(F86:F88,"Y"),COUNTIF(F106:F108,"Y"),COUNTIF(F126:F128,"Y"))
+/
+SUM(COUNTIF(F21:F23,"Y"),COUNTIF(F21:F23,"N"),COUNTIF(F44:F46,"Y"),COUNTIF(F44:F46,"N"),COUNTIF(F65:F67,"Y"),COUNTIF(F65:F67,"N"),COUNTIF(F86:F88,"Y"),COUNTIF(F86:F88,"N"),COUNTIF(F106:F108,"Y"),COUNTIF(F106:F108,"N"),COUNTIF(F126:F128,"Y"),COUNTIF(F126:F128,"N"))</f>
+        <v>1</v>
+      </c>
+      <c r="G158" s="26">
+        <f t="shared" ref="G158:N158" si="64">SUM(COUNTIF(G21:G23,"Y"),COUNTIF(G44:G46,"Y"),COUNTIF(G65:G67,"Y"),COUNTIF(G86:G88,"Y"),COUNTIF(G106:G108,"Y"),COUNTIF(G126:G128,"Y"))
+/
+SUM(COUNTIF(G21:G23,"Y"),COUNTIF(G21:G23,"N"),COUNTIF(G44:G46,"Y"),COUNTIF(G44:G46,"N"),COUNTIF(G65:G67,"Y"),COUNTIF(G65:G67,"N"),COUNTIF(G86:G88,"Y"),COUNTIF(G86:G88,"N"),COUNTIF(G106:G108,"Y"),COUNTIF(G106:G108,"N"),COUNTIF(G126:G128,"Y"),COUNTIF(G126:G128,"N"))</f>
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="H158" s="26">
+        <f t="shared" si="64"/>
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="I158" s="26">
+        <f t="shared" si="64"/>
         <v>0.5</v>
       </c>
-      <c r="J158">
+      <c r="J158" s="26">
+        <f t="shared" si="64"/>
         <v>0.5</v>
       </c>
-      <c r="L158">
+      <c r="K158" s="26"/>
+      <c r="L158" s="26">
+        <f t="shared" si="64"/>
         <v>0.5</v>
       </c>
-      <c r="M158">
-        <v>0.38888888900000002</v>
-      </c>
-      <c r="N158">
-        <v>0.38888888900000002</v>
-      </c>
-    </row>
-    <row r="159" spans="4:27" x14ac:dyDescent="0.3">
-      <c r="D159" t="s">
+      <c r="M158" s="26">
+        <f t="shared" si="64"/>
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="N158" s="27">
+        <f t="shared" si="64"/>
+        <v>0.3888888888888889</v>
+      </c>
+    </row>
+    <row r="164" spans="4:14" x14ac:dyDescent="0.3">
+      <c r="D164" t="s">
         <v>44</v>
       </c>
-      <c r="E159" t="s">
+      <c r="E164" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="160" spans="4:27" x14ac:dyDescent="0.3">
-      <c r="D160">
-        <v>0</v>
-      </c>
-      <c r="F160">
-        <v>0</v>
-      </c>
-      <c r="G160">
+      <c r="G164" s="12"/>
+      <c r="H164" s="12"/>
+      <c r="I164" s="12"/>
+      <c r="J164" s="12"/>
+      <c r="K164" s="12"/>
+      <c r="L164" s="12"/>
+      <c r="M164" s="12"/>
+      <c r="N164" s="12"/>
+    </row>
+    <row r="165" spans="4:14" x14ac:dyDescent="0.3">
+      <c r="D165">
+        <v>0</v>
+      </c>
+      <c r="F165">
+        <v>0</v>
+      </c>
+      <c r="G165" s="12">
         <v>0.403686714</v>
       </c>
-      <c r="H160">
+      <c r="H165" s="12">
         <v>0.51639777899999995</v>
       </c>
-      <c r="I160">
+      <c r="I165" s="12">
         <v>0.40824829000000001</v>
       </c>
-      <c r="J160">
+      <c r="J165" s="12">
         <v>0.51639777899999995</v>
       </c>
-      <c r="L160">
+      <c r="K165" s="12"/>
+      <c r="L165" s="12">
         <v>0.421637021</v>
       </c>
-      <c r="M160">
+      <c r="M165" s="12">
         <v>0.421637021</v>
       </c>
-      <c r="N160">
+      <c r="N165" s="12">
         <v>0.50184843499999998</v>
       </c>
     </row>
-    <row r="161" spans="4:14" x14ac:dyDescent="0.3">
-      <c r="D161">
+    <row r="166" spans="4:14" x14ac:dyDescent="0.3">
+      <c r="D166">
         <v>0.3</v>
       </c>
-      <c r="F161">
-        <v>0</v>
-      </c>
-      <c r="G161">
+      <c r="F166">
+        <v>0</v>
+      </c>
+      <c r="G166" s="12">
         <v>0.40824829000000001</v>
       </c>
-      <c r="H161">
+      <c r="H166" s="12">
         <v>0.44305337900000002</v>
       </c>
-      <c r="I161">
+      <c r="I166" s="12">
         <v>0.25092421799999998</v>
       </c>
-      <c r="J161">
+      <c r="J166" s="12">
         <v>0.45542003399999997</v>
       </c>
-      <c r="L161">
+      <c r="K166" s="12"/>
+      <c r="L166" s="12">
         <v>0.344265186</v>
       </c>
-      <c r="M161">
+      <c r="M166" s="12">
         <v>0.349602949</v>
       </c>
-      <c r="N161">
+      <c r="N166" s="12">
         <v>0.349602949</v>
       </c>
     </row>
-    <row r="162" spans="4:14" x14ac:dyDescent="0.3">
-      <c r="D162">
+    <row r="167" spans="4:14" x14ac:dyDescent="0.3">
+      <c r="D167">
         <v>0.7</v>
       </c>
-      <c r="F162">
-        <v>0</v>
-      </c>
-      <c r="G162">
+      <c r="F167">
+        <v>0</v>
+      </c>
+      <c r="G167" s="12">
         <v>0.403686714</v>
       </c>
-      <c r="H162">
+      <c r="H167" s="12">
         <v>0.278886676</v>
       </c>
-      <c r="I162">
+      <c r="I167" s="12">
         <v>0.27216552700000002</v>
       </c>
-      <c r="J162">
+      <c r="J167" s="12">
         <v>0.403686714</v>
       </c>
-      <c r="L162">
+      <c r="K167" s="12"/>
+      <c r="L167" s="12">
         <v>0.421637021</v>
       </c>
-      <c r="M162">
+      <c r="M167" s="12">
         <v>0.403686714</v>
       </c>
-      <c r="N162">
+      <c r="N167" s="12">
         <v>0.365148372</v>
       </c>
     </row>
-    <row r="163" spans="4:14" x14ac:dyDescent="0.3">
-      <c r="D163">
-        <v>1</v>
-      </c>
-      <c r="F163">
-        <v>0</v>
-      </c>
-      <c r="G163">
+    <row r="168" spans="4:14" x14ac:dyDescent="0.3">
+      <c r="D168">
+        <v>1</v>
+      </c>
+      <c r="F168">
+        <v>0</v>
+      </c>
+      <c r="G168" s="12">
         <v>0.172132593</v>
       </c>
-      <c r="H163">
+      <c r="H168" s="12">
         <v>0.27216552700000002</v>
       </c>
-      <c r="I163">
+      <c r="I168" s="12">
         <v>0.40824829000000001</v>
       </c>
-      <c r="J163">
+      <c r="J168" s="12">
         <v>0.40824829000000001</v>
       </c>
-      <c r="L163">
+      <c r="K168" s="12"/>
+      <c r="L168" s="12">
         <v>0.349602949</v>
       </c>
-      <c r="M163">
+      <c r="M168" s="12">
         <v>0.25092421799999998</v>
       </c>
-      <c r="N163">
+      <c r="N168" s="12">
         <v>0.32773069300000002</v>
       </c>
     </row>
@@ -13012,6 +13672,10 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="W143:AA143"/>
+    <mergeCell ref="E153:N153"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>